<commit_message>
added staging table for cineas-hpo mappings
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="153">
   <si>
     <t>cosasportal</t>
   </si>
@@ -24,7 +24,7 @@
     <t>COSAS Portal</t>
   </si>
   <si>
-    <t>Staging tables for raw data exports (v1.2.0, 2022-02-10)</t>
+    <t>Staging tables for raw data exports (v1.3.0, 2022-02-17)</t>
   </si>
   <si>
     <t>template</t>
@@ -54,6 +54,9 @@
     <t>benchcnv</t>
   </si>
   <si>
+    <t>cineasmappings</t>
+  </si>
+  <si>
     <t>attribute template for staging tables</t>
   </si>
   <si>
@@ -81,6 +84,9 @@
     <t>Staging table for CNV exports</t>
   </si>
   <si>
+    <t>Cineas to HPO mappings</t>
+  </si>
+  <si>
     <t>cosasportal_template</t>
   </si>
   <si>
@@ -108,6 +114,9 @@
     <t>cosasportal_benchcnv</t>
   </si>
   <si>
+    <t>cosasportal_cineasmappings</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -378,6 +387,21 @@
     <t>created</t>
   </si>
   <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>codesystem</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>hpo</t>
+  </si>
+  <si>
     <t>auto generated row identifier</t>
   </si>
   <si>
@@ -418,9 +442,6 @@
   </si>
   <si>
     <t>label</t>
-  </si>
-  <si>
-    <t>description</t>
   </si>
   <si>
     <t>package</t>
@@ -808,13 +829,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -835,7 +856,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -843,19 +864,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -866,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -880,10 +901,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -894,10 +915,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -908,10 +929,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -922,10 +943,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -936,10 +957,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -950,10 +971,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -964,10 +985,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -978,10 +999,21 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -991,7 +1023,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -999,45 +1031,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1052,18 +1084,18 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1078,18 +1110,18 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1104,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -1112,13 +1144,13 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1133,47 +1165,47 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1188,15 +1220,15 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1211,15 +1243,15 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -1234,15 +1266,15 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -1257,15 +1289,15 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1280,15 +1312,15 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1303,15 +1335,15 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1326,15 +1358,15 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1349,15 +1381,15 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1372,15 +1404,15 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1395,15 +1427,15 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -1418,15 +1450,15 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1441,15 +1473,15 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -1464,15 +1496,15 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1487,15 +1519,15 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -1510,15 +1542,15 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1533,15 +1565,15 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -1556,15 +1588,15 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -1579,15 +1611,15 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -1602,15 +1634,15 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -1625,15 +1657,15 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -1648,15 +1680,15 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1671,15 +1703,15 @@
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -1694,15 +1726,15 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -1717,15 +1749,15 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -1740,15 +1772,15 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -1763,15 +1795,15 @@
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -1786,15 +1818,15 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -1809,15 +1841,15 @@
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -1832,15 +1864,15 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -1855,15 +1887,15 @@
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -1878,15 +1910,15 @@
         <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -1901,15 +1933,15 @@
         <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -1924,15 +1956,15 @@
         <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -1947,15 +1979,15 @@
         <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -1970,15 +2002,15 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -1993,15 +2025,15 @@
         <v>0</v>
       </c>
       <c r="H42" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -2016,15 +2048,15 @@
         <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -2039,15 +2071,15 @@
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -2062,15 +2094,15 @@
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2085,15 +2117,15 @@
         <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -2108,15 +2140,15 @@
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -2131,15 +2163,15 @@
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -2154,15 +2186,15 @@
         <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -2177,15 +2209,15 @@
         <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -2200,15 +2232,15 @@
         <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -2223,15 +2255,15 @@
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -2246,15 +2278,15 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -2269,15 +2301,15 @@
         <v>0</v>
       </c>
       <c r="H54" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -2292,15 +2324,15 @@
         <v>0</v>
       </c>
       <c r="H55" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -2315,15 +2347,15 @@
         <v>0</v>
       </c>
       <c r="H56" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -2338,15 +2370,15 @@
         <v>0</v>
       </c>
       <c r="H57" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -2361,15 +2393,15 @@
         <v>0</v>
       </c>
       <c r="H58" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -2384,15 +2416,15 @@
         <v>0</v>
       </c>
       <c r="H59" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -2407,15 +2439,15 @@
         <v>0</v>
       </c>
       <c r="H60" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -2430,15 +2462,15 @@
         <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -2453,15 +2485,15 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -2476,15 +2508,15 @@
         <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B64" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -2499,15 +2531,15 @@
         <v>0</v>
       </c>
       <c r="H64" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -2522,15 +2554,15 @@
         <v>0</v>
       </c>
       <c r="H65" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -2545,15 +2577,15 @@
         <v>0</v>
       </c>
       <c r="H66" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -2568,15 +2600,15 @@
         <v>0</v>
       </c>
       <c r="H67" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -2591,15 +2623,15 @@
         <v>0</v>
       </c>
       <c r="H68" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B69" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -2614,15 +2646,15 @@
         <v>0</v>
       </c>
       <c r="H69" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -2637,15 +2669,15 @@
         <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -2660,15 +2692,15 @@
         <v>0</v>
       </c>
       <c r="H71" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -2683,15 +2715,15 @@
         <v>0</v>
       </c>
       <c r="H72" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -2706,15 +2738,15 @@
         <v>0</v>
       </c>
       <c r="H73" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -2729,15 +2761,15 @@
         <v>0</v>
       </c>
       <c r="H74" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -2752,15 +2784,15 @@
         <v>0</v>
       </c>
       <c r="H75" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -2775,15 +2807,15 @@
         <v>0</v>
       </c>
       <c r="H76" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -2798,15 +2830,15 @@
         <v>0</v>
       </c>
       <c r="H77" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
@@ -2821,15 +2853,15 @@
         <v>0</v>
       </c>
       <c r="H78" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D79" t="b">
         <v>0</v>
@@ -2844,15 +2876,15 @@
         <v>0</v>
       </c>
       <c r="H79" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B80" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
@@ -2867,15 +2899,15 @@
         <v>0</v>
       </c>
       <c r="H80" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B81" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -2890,15 +2922,15 @@
         <v>0</v>
       </c>
       <c r="H81" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B82" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
@@ -2913,15 +2945,15 @@
         <v>0</v>
       </c>
       <c r="H82" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
@@ -2936,15 +2968,15 @@
         <v>0</v>
       </c>
       <c r="H83" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B84" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
@@ -2959,15 +2991,15 @@
         <v>0</v>
       </c>
       <c r="H84" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -2982,15 +3014,15 @@
         <v>0</v>
       </c>
       <c r="H85" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D86" t="b">
         <v>0</v>
@@ -3005,15 +3037,15 @@
         <v>0</v>
       </c>
       <c r="H86" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
@@ -3028,15 +3060,15 @@
         <v>0</v>
       </c>
       <c r="H87" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
@@ -3051,15 +3083,15 @@
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -3074,15 +3106,15 @@
         <v>0</v>
       </c>
       <c r="H89" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B90" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D90" t="b">
         <v>0</v>
@@ -3097,15 +3129,15 @@
         <v>0</v>
       </c>
       <c r="H90" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B91" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
@@ -3120,15 +3152,15 @@
         <v>0</v>
       </c>
       <c r="H91" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B92" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D92" t="b">
         <v>0</v>
@@ -3143,15 +3175,15 @@
         <v>0</v>
       </c>
       <c r="H92" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B93" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D93" t="b">
         <v>0</v>
@@ -3166,15 +3198,15 @@
         <v>0</v>
       </c>
       <c r="H93" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B94" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D94" t="b">
         <v>0</v>
@@ -3189,15 +3221,15 @@
         <v>0</v>
       </c>
       <c r="H94" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D95" t="b">
         <v>0</v>
@@ -3212,15 +3244,15 @@
         <v>0</v>
       </c>
       <c r="H95" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D96" t="b">
         <v>0</v>
@@ -3235,15 +3267,15 @@
         <v>0</v>
       </c>
       <c r="H96" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B97" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D97" t="b">
         <v>0</v>
@@ -3258,15 +3290,15 @@
         <v>0</v>
       </c>
       <c r="H97" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
@@ -3281,15 +3313,15 @@
         <v>0</v>
       </c>
       <c r="H98" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B99" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D99" t="b">
         <v>0</v>
@@ -3304,15 +3336,15 @@
         <v>0</v>
       </c>
       <c r="H99" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B100" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D100" t="b">
         <v>0</v>
@@ -3327,15 +3359,15 @@
         <v>0</v>
       </c>
       <c r="H100" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B101" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D101" t="b">
         <v>0</v>
@@ -3350,15 +3382,15 @@
         <v>0</v>
       </c>
       <c r="H101" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D102" t="b">
         <v>0</v>
@@ -3373,15 +3405,15 @@
         <v>0</v>
       </c>
       <c r="H102" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B103" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D103" t="b">
         <v>0</v>
@@ -3396,18 +3428,18 @@
         <v>0</v>
       </c>
       <c r="H103" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B104" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C104" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -3422,18 +3454,18 @@
         <v>0</v>
       </c>
       <c r="H104" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B105" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C105" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D105" t="b">
         <v>0</v>
@@ -3448,15 +3480,15 @@
         <v>0</v>
       </c>
       <c r="H105" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D106" t="b">
         <v>0</v>
@@ -3471,15 +3503,15 @@
         <v>0</v>
       </c>
       <c r="H106" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D107" t="b">
         <v>0</v>
@@ -3494,15 +3526,15 @@
         <v>0</v>
       </c>
       <c r="H107" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B108" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D108" t="b">
         <v>0</v>
@@ -3517,15 +3549,15 @@
         <v>0</v>
       </c>
       <c r="H108" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D109" t="b">
         <v>0</v>
@@ -3540,15 +3572,15 @@
         <v>0</v>
       </c>
       <c r="H109" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="110" spans="1:8">
       <c r="A110" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B110" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D110" t="b">
         <v>0</v>
@@ -3563,7 +3595,122 @@
         <v>0</v>
       </c>
       <c r="H110" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>32</v>
+      </c>
+      <c r="B111" t="s">
+        <v>123</v>
+      </c>
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111" t="b">
+        <v>0</v>
+      </c>
+      <c r="G111" t="b">
+        <v>0</v>
+      </c>
+      <c r="H111" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>32</v>
+      </c>
+      <c r="B112" t="s">
+        <v>124</v>
+      </c>
+      <c r="D112" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112" t="b">
+        <v>1</v>
+      </c>
+      <c r="G112" t="b">
+        <v>0</v>
+      </c>
+      <c r="H112" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" t="s">
+        <v>32</v>
+      </c>
+      <c r="B113" t="s">
+        <v>125</v>
+      </c>
+      <c r="D113" t="b">
+        <v>0</v>
+      </c>
+      <c r="E113" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>32</v>
+      </c>
+      <c r="B114" t="s">
+        <v>126</v>
+      </c>
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" t="b">
+        <v>1</v>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+      <c r="H114" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>32</v>
+      </c>
+      <c r="B115" t="s">
         <v>127</v>
+      </c>
+      <c r="D115" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" t="b">
+        <v>1</v>
+      </c>
+      <c r="G115" t="b">
+        <v>0</v>
+      </c>
+      <c r="H115" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added prepped table for cnv data
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="162">
   <si>
     <t>cosasportal</t>
   </si>
@@ -24,7 +24,7 @@
     <t>COSAS Portal</t>
   </si>
   <si>
-    <t>Staging tables for raw data exports (v1.4.0, 2022-02-21)</t>
+    <t>Staging tables for raw data exports (v1.5.0, 2022-02-21)</t>
   </si>
   <si>
     <t>template</t>
@@ -54,6 +54,9 @@
     <t>benchcnv</t>
   </si>
   <si>
+    <t>benchcnv_prepped</t>
+  </si>
+  <si>
     <t>cineasmappings</t>
   </si>
   <si>
@@ -81,7 +84,10 @@
     <t>Raw NSG metadata from Darwin</t>
   </si>
   <si>
-    <t>Staging table for CNV exports</t>
+    <t>Staging table for Raw CNV exports</t>
+  </si>
+  <si>
+    <t>Processed CNV bench data</t>
   </si>
   <si>
     <t>Cineas to HPO mappings</t>
@@ -114,6 +120,9 @@
     <t>cosasportal_benchcnv</t>
   </si>
   <si>
+    <t>cosasportal_benchcnv_prepped</t>
+  </si>
+  <si>
     <t>cosasportal_cineasmappings</t>
   </si>
   <si>
@@ -385,6 +394,24 @@
   </si>
   <si>
     <t>created</t>
+  </si>
+  <si>
+    <t>subjectID</t>
+  </si>
+  <si>
+    <t>belongsToMother</t>
+  </si>
+  <si>
+    <t>belongsToFamily</t>
+  </si>
+  <si>
+    <t>isFetus</t>
+  </si>
+  <si>
+    <t>alternativeIdentifiers</t>
+  </si>
+  <si>
+    <t>observedPhenotype</t>
   </si>
   <si>
     <t>value</t>
@@ -829,13 +856,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -856,7 +883,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -864,19 +891,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -887,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -901,10 +928,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -915,10 +942,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -929,10 +956,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -943,10 +970,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -957,10 +984,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -971,10 +998,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -985,10 +1012,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -999,10 +1026,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1013,7 +1040,21 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1064,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1031,45 +1072,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1084,18 +1125,18 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1110,18 +1151,18 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1136,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -1144,13 +1185,13 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1165,47 +1206,47 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J6" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>135</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1220,15 +1261,15 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1243,15 +1284,15 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -1266,15 +1307,15 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -1289,15 +1330,15 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1312,15 +1353,15 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1335,15 +1376,15 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1358,15 +1399,15 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1381,15 +1422,15 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1404,15 +1445,15 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1427,15 +1468,15 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -1450,15 +1491,15 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1473,15 +1514,15 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -1496,15 +1537,15 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1519,15 +1560,15 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -1542,15 +1583,15 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1565,15 +1606,15 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -1588,15 +1629,15 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -1611,15 +1652,15 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -1634,15 +1675,15 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -1657,15 +1698,15 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -1680,15 +1721,15 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1703,15 +1744,15 @@
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -1726,15 +1767,15 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -1749,15 +1790,15 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -1772,15 +1813,15 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -1795,15 +1836,15 @@
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -1818,15 +1859,15 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -1841,15 +1882,15 @@
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -1864,15 +1905,15 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -1887,15 +1928,15 @@
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -1910,15 +1951,15 @@
         <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -1933,15 +1974,15 @@
         <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -1956,15 +1997,15 @@
         <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -1979,15 +2020,15 @@
         <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -2002,15 +2043,15 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -2025,15 +2066,15 @@
         <v>0</v>
       </c>
       <c r="H42" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -2048,15 +2089,15 @@
         <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -2071,15 +2112,15 @@
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -2094,15 +2135,15 @@
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2117,15 +2158,15 @@
         <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -2140,15 +2181,15 @@
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -2163,15 +2204,15 @@
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -2186,15 +2227,15 @@
         <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -2209,15 +2250,15 @@
         <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -2232,15 +2273,15 @@
         <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -2255,15 +2296,15 @@
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -2278,15 +2319,15 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -2301,15 +2342,15 @@
         <v>0</v>
       </c>
       <c r="H54" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -2324,15 +2365,15 @@
         <v>0</v>
       </c>
       <c r="H55" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -2347,15 +2388,15 @@
         <v>0</v>
       </c>
       <c r="H56" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -2370,15 +2411,15 @@
         <v>0</v>
       </c>
       <c r="H57" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -2393,15 +2434,15 @@
         <v>0</v>
       </c>
       <c r="H58" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -2416,15 +2457,15 @@
         <v>0</v>
       </c>
       <c r="H59" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -2439,15 +2480,15 @@
         <v>0</v>
       </c>
       <c r="H60" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -2462,15 +2503,15 @@
         <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -2485,15 +2526,15 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -2508,15 +2549,15 @@
         <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -2531,15 +2572,15 @@
         <v>0</v>
       </c>
       <c r="H64" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -2554,15 +2595,15 @@
         <v>0</v>
       </c>
       <c r="H65" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -2577,15 +2618,15 @@
         <v>0</v>
       </c>
       <c r="H66" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -2600,15 +2641,15 @@
         <v>0</v>
       </c>
       <c r="H67" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B68" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -2623,15 +2664,15 @@
         <v>0</v>
       </c>
       <c r="H68" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -2646,15 +2687,15 @@
         <v>0</v>
       </c>
       <c r="H69" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -2669,15 +2710,15 @@
         <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -2692,15 +2733,15 @@
         <v>0</v>
       </c>
       <c r="H71" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -2715,15 +2756,15 @@
         <v>0</v>
       </c>
       <c r="H72" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -2738,15 +2779,15 @@
         <v>0</v>
       </c>
       <c r="H73" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -2761,15 +2802,15 @@
         <v>0</v>
       </c>
       <c r="H74" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -2784,15 +2825,15 @@
         <v>0</v>
       </c>
       <c r="H75" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -2807,15 +2848,15 @@
         <v>0</v>
       </c>
       <c r="H76" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -2830,15 +2871,15 @@
         <v>0</v>
       </c>
       <c r="H77" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
@@ -2853,15 +2894,15 @@
         <v>0</v>
       </c>
       <c r="H78" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D79" t="b">
         <v>0</v>
@@ -2876,15 +2917,15 @@
         <v>0</v>
       </c>
       <c r="H79" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
@@ -2899,15 +2940,15 @@
         <v>0</v>
       </c>
       <c r="H80" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B81" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -2922,15 +2963,15 @@
         <v>0</v>
       </c>
       <c r="H81" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B82" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
@@ -2945,15 +2986,15 @@
         <v>0</v>
       </c>
       <c r="H82" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
@@ -2968,15 +3009,15 @@
         <v>0</v>
       </c>
       <c r="H83" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
@@ -2991,15 +3032,15 @@
         <v>0</v>
       </c>
       <c r="H84" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -3014,15 +3055,15 @@
         <v>0</v>
       </c>
       <c r="H85" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B86" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D86" t="b">
         <v>0</v>
@@ -3037,15 +3078,15 @@
         <v>0</v>
       </c>
       <c r="H86" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
@@ -3060,15 +3101,15 @@
         <v>0</v>
       </c>
       <c r="H87" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B88" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
@@ -3083,15 +3124,15 @@
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -3106,15 +3147,15 @@
         <v>0</v>
       </c>
       <c r="H89" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B90" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D90" t="b">
         <v>0</v>
@@ -3129,15 +3170,15 @@
         <v>0</v>
       </c>
       <c r="H90" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
@@ -3152,15 +3193,15 @@
         <v>0</v>
       </c>
       <c r="H91" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D92" t="b">
         <v>0</v>
@@ -3175,15 +3216,15 @@
         <v>0</v>
       </c>
       <c r="H92" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D93" t="b">
         <v>0</v>
@@ -3198,15 +3239,15 @@
         <v>0</v>
       </c>
       <c r="H93" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D94" t="b">
         <v>0</v>
@@ -3221,15 +3262,15 @@
         <v>0</v>
       </c>
       <c r="H94" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D95" t="b">
         <v>0</v>
@@ -3244,15 +3285,15 @@
         <v>0</v>
       </c>
       <c r="H95" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D96" t="b">
         <v>0</v>
@@ -3267,15 +3308,15 @@
         <v>0</v>
       </c>
       <c r="H96" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D97" t="b">
         <v>0</v>
@@ -3290,15 +3331,15 @@
         <v>0</v>
       </c>
       <c r="H97" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
@@ -3313,15 +3354,15 @@
         <v>0</v>
       </c>
       <c r="H98" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D99" t="b">
         <v>0</v>
@@ -3336,15 +3377,15 @@
         <v>0</v>
       </c>
       <c r="H99" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D100" t="b">
         <v>0</v>
@@ -3359,15 +3400,15 @@
         <v>0</v>
       </c>
       <c r="H100" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D101" t="b">
         <v>0</v>
@@ -3382,15 +3423,15 @@
         <v>0</v>
       </c>
       <c r="H101" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D102" t="b">
         <v>0</v>
@@ -3405,15 +3446,15 @@
         <v>0</v>
       </c>
       <c r="H102" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D103" t="b">
         <v>0</v>
@@ -3428,18 +3469,18 @@
         <v>0</v>
       </c>
       <c r="H103" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C104" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -3454,18 +3495,18 @@
         <v>0</v>
       </c>
       <c r="H104" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C105" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="D105" t="b">
         <v>0</v>
@@ -3480,15 +3521,15 @@
         <v>0</v>
       </c>
       <c r="H105" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D106" t="b">
         <v>0</v>
@@ -3503,15 +3544,15 @@
         <v>0</v>
       </c>
       <c r="H106" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B107" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D107" t="b">
         <v>0</v>
@@ -3526,15 +3567,15 @@
         <v>0</v>
       </c>
       <c r="H107" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D108" t="b">
         <v>0</v>
@@ -3549,15 +3590,15 @@
         <v>0</v>
       </c>
       <c r="H108" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B109" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D109" t="b">
         <v>0</v>
@@ -3572,15 +3613,15 @@
         <v>0</v>
       </c>
       <c r="H109" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:8">
       <c r="A110" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B110" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D110" t="b">
         <v>0</v>
@@ -3595,38 +3636,38 @@
         <v>0</v>
       </c>
       <c r="H110" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:8">
       <c r="A111" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B111" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111" t="b">
         <v>0</v>
       </c>
       <c r="F111" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G111" t="b">
         <v>0</v>
       </c>
       <c r="H111" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D112" t="b">
         <v>0</v>
@@ -3641,15 +3682,15 @@
         <v>0</v>
       </c>
       <c r="H112" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B113" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D113" t="b">
         <v>0</v>
@@ -3664,15 +3705,15 @@
         <v>0</v>
       </c>
       <c r="H113" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B114" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D114" t="b">
         <v>0</v>
@@ -3687,15 +3728,15 @@
         <v>0</v>
       </c>
       <c r="H114" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="115" spans="1:8">
       <c r="A115" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B115" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D115" t="b">
         <v>0</v>
@@ -3710,7 +3751,168 @@
         <v>0</v>
       </c>
       <c r="H115" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" t="s">
+        <v>34</v>
+      </c>
+      <c r="B116" t="s">
+        <v>130</v>
+      </c>
+      <c r="D116" t="b">
+        <v>0</v>
+      </c>
+      <c r="E116" t="b">
+        <v>0</v>
+      </c>
+      <c r="F116" t="b">
+        <v>1</v>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+      <c r="H116" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B117" t="s">
+        <v>131</v>
+      </c>
+      <c r="D117" t="b">
+        <v>0</v>
+      </c>
+      <c r="E117" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" t="b">
+        <v>1</v>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+      <c r="H117" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" t="s">
+        <v>35</v>
+      </c>
+      <c r="B118" t="s">
+        <v>132</v>
+      </c>
+      <c r="D118" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118" t="b">
+        <v>0</v>
+      </c>
+      <c r="G118" t="b">
+        <v>0</v>
+      </c>
+      <c r="H118" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>35</v>
+      </c>
+      <c r="B119" t="s">
+        <v>133</v>
+      </c>
+      <c r="D119" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" t="b">
+        <v>1</v>
+      </c>
+      <c r="G119" t="b">
+        <v>0</v>
+      </c>
+      <c r="H119" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" t="s">
+        <v>35</v>
+      </c>
+      <c r="B120" t="s">
+        <v>134</v>
+      </c>
+      <c r="D120" t="b">
+        <v>0</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" t="b">
+        <v>1</v>
+      </c>
+      <c r="G120" t="b">
+        <v>0</v>
+      </c>
+      <c r="H120" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="s">
+        <v>35</v>
+      </c>
+      <c r="B121" t="s">
         <v>135</v>
+      </c>
+      <c r="D121" t="b">
+        <v>0</v>
+      </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" t="b">
+        <v>1</v>
+      </c>
+      <c r="G121" t="b">
+        <v>0</v>
+      </c>
+      <c r="H121" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" t="s">
+        <v>35</v>
+      </c>
+      <c r="B122" t="s">
+        <v>136</v>
+      </c>
+      <c r="D122" t="b">
+        <v>0</v>
+      </c>
+      <c r="E122" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122" t="b">
+        <v>1</v>
+      </c>
+      <c r="G122" t="b">
+        <v>0</v>
+      </c>
+      <c r="H122" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rebuild model and schemas
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -10,13 +10,14 @@
     <sheet name="packages" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
+    <sheet name="tags" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="206">
   <si>
     <t>cosasportal</t>
   </si>
@@ -33,7 +34,7 @@
     <t>Staging tables for raw data exports (v1.6.0, 2022-03-28)</t>
   </si>
   <si>
-    <t>Mapping tables for processing raw data into UMDM terminology</t>
+    <t>Mapping tables for processing raw data into UMDM terminology (v1.0.0, 2022-03-29)</t>
   </si>
   <si>
     <t>template</t>
@@ -444,13 +445,13 @@
     <t>hpo</t>
   </si>
   <si>
-    <t>sourceValue</t>
-  </si>
-  <si>
-    <t>newValue</t>
-  </si>
-  <si>
-    <t>newValueSecondary</t>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>toAlternate</t>
   </si>
   <si>
     <t>auto generated row identifier</t>
@@ -489,13 +490,37 @@
     <t>HPO terms provided by Cartagenia</t>
   </si>
   <si>
-    <t>Value as listed in the data export</t>
-  </si>
-  <si>
-    <t>New value to assign</t>
-  </si>
-  <si>
-    <t>A secondary value that corresponds to the source value</t>
+    <t>Used to indicate a specified place or time as a starting point; used to indicate a source, cause, agent, or instrument.</t>
+  </si>
+  <si>
+    <t>Used as a function word to indicate direction, purpose, or movement.</t>
+  </si>
+  <si>
+    <t>Available in place of something else.</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001330</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#ProcessedData</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25516</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C65107</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25415</t>
   </si>
   <si>
     <t>string</t>
@@ -546,6 +571,9 @@
     <t>lookupAttribute</t>
   </si>
   <si>
+    <t>tags</t>
+  </si>
+  <si>
     <t>dataType</t>
   </si>
   <si>
@@ -553,13 +581,67 @@
   </si>
   <si>
     <t>partOfAttribute</t>
+  </si>
+  <si>
+    <t>NCIT:C164483</t>
+  </si>
+  <si>
+    <t>NCIT:C25364</t>
+  </si>
+  <si>
+    <t>NCIT:C25415</t>
+  </si>
+  <si>
+    <t>NCIT:C25516</t>
+  </si>
+  <si>
+    <t>NCIT:C42628</t>
+  </si>
+  <si>
+    <t>NCIT:C65107</t>
+  </si>
+  <si>
+    <t>SIO:001330</t>
+  </si>
+  <si>
+    <t>W3ID:ProcessedData</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>SIO</t>
+  </si>
+  <si>
+    <t>W3ID</t>
+  </si>
+  <si>
+    <t>isAssociatedWith</t>
+  </si>
+  <si>
+    <t>http://molgenis.org#isAssociatedWith</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>objectIRI</t>
+  </si>
+  <si>
+    <t>codeSystem</t>
+  </si>
+  <si>
+    <t>relationLabel</t>
+  </si>
+  <si>
+    <t>relationIRI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +655,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -599,14 +688,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -907,16 +1002,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -959,19 +1054,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1199,45 +1294,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>186</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1259,11 +1357,14 @@
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="I2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1285,11 +1386,14 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="I3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1311,14 +1415,17 @@
       <c r="G4" t="b">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="I4" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1340,14 +1447,17 @@
       <c r="G5" t="b">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" t="s">
+        <v>171</v>
+      </c>
+      <c r="K5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1369,14 +1479,17 @@
       <c r="G6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
-        <v>160</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="H6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I6" t="s">
+        <v>168</v>
+      </c>
+      <c r="K6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1395,11 +1508,11 @@
       <c r="G7" t="b">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="I7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1418,11 +1531,11 @@
       <c r="G8" t="b">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="I8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1441,11 +1554,11 @@
       <c r="G9" t="b">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="I9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1464,11 +1577,11 @@
       <c r="G10" t="b">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="I10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1487,11 +1600,11 @@
       <c r="G11" t="b">
         <v>0</v>
       </c>
-      <c r="H11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="I11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1510,11 +1623,11 @@
       <c r="G12" t="b">
         <v>0</v>
       </c>
-      <c r="H12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="I12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1533,11 +1646,11 @@
       <c r="G13" t="b">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="I13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1556,11 +1669,11 @@
       <c r="G14" t="b">
         <v>0</v>
       </c>
-      <c r="H14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="I14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1579,11 +1692,11 @@
       <c r="G15" t="b">
         <v>0</v>
       </c>
-      <c r="H15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="I15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1602,11 +1715,11 @@
       <c r="G16" t="b">
         <v>0</v>
       </c>
-      <c r="H16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1625,11 +1738,11 @@
       <c r="G17" t="b">
         <v>0</v>
       </c>
-      <c r="H17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1648,11 +1761,11 @@
       <c r="G18" t="b">
         <v>0</v>
       </c>
-      <c r="H18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1671,11 +1784,11 @@
       <c r="G19" t="b">
         <v>0</v>
       </c>
-      <c r="H19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1694,11 +1807,11 @@
       <c r="G20" t="b">
         <v>0</v>
       </c>
-      <c r="H20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1717,11 +1830,11 @@
       <c r="G21" t="b">
         <v>0</v>
       </c>
-      <c r="H21" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1740,11 +1853,11 @@
       <c r="G22" t="b">
         <v>0</v>
       </c>
-      <c r="H22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1763,11 +1876,11 @@
       <c r="G23" t="b">
         <v>0</v>
       </c>
-      <c r="H23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1786,11 +1899,11 @@
       <c r="G24" t="b">
         <v>0</v>
       </c>
-      <c r="H24" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1809,11 +1922,11 @@
       <c r="G25" t="b">
         <v>0</v>
       </c>
-      <c r="H25" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1832,11 +1945,11 @@
       <c r="G26" t="b">
         <v>0</v>
       </c>
-      <c r="H26" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1855,11 +1968,11 @@
       <c r="G27" t="b">
         <v>0</v>
       </c>
-      <c r="H27" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1878,11 +1991,11 @@
       <c r="G28" t="b">
         <v>0</v>
       </c>
-      <c r="H28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1901,11 +2014,11 @@
       <c r="G29" t="b">
         <v>0</v>
       </c>
-      <c r="H29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1924,11 +2037,11 @@
       <c r="G30" t="b">
         <v>0</v>
       </c>
-      <c r="H30" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1947,11 +2060,11 @@
       <c r="G31" t="b">
         <v>0</v>
       </c>
-      <c r="H31" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1970,11 +2083,11 @@
       <c r="G32" t="b">
         <v>0</v>
       </c>
-      <c r="H32" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1993,11 +2106,11 @@
       <c r="G33" t="b">
         <v>0</v>
       </c>
-      <c r="H33" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2016,11 +2129,11 @@
       <c r="G34" t="b">
         <v>0</v>
       </c>
-      <c r="H34" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2039,11 +2152,11 @@
       <c r="G35" t="b">
         <v>0</v>
       </c>
-      <c r="H35" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2062,11 +2175,11 @@
       <c r="G36" t="b">
         <v>0</v>
       </c>
-      <c r="H36" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2085,11 +2198,11 @@
       <c r="G37" t="b">
         <v>0</v>
       </c>
-      <c r="H37" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2108,11 +2221,11 @@
       <c r="G38" t="b">
         <v>0</v>
       </c>
-      <c r="H38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2131,11 +2244,11 @@
       <c r="G39" t="b">
         <v>0</v>
       </c>
-      <c r="H39" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -2154,11 +2267,11 @@
       <c r="G40" t="b">
         <v>0</v>
       </c>
-      <c r="H40" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2177,11 +2290,11 @@
       <c r="G41" t="b">
         <v>0</v>
       </c>
-      <c r="H41" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2200,11 +2313,11 @@
       <c r="G42" t="b">
         <v>0</v>
       </c>
-      <c r="H42" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2223,11 +2336,11 @@
       <c r="G43" t="b">
         <v>0</v>
       </c>
-      <c r="H43" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2246,11 +2359,11 @@
       <c r="G44" t="b">
         <v>0</v>
       </c>
-      <c r="H44" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -2269,11 +2382,11 @@
       <c r="G45" t="b">
         <v>0</v>
       </c>
-      <c r="H45" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -2292,11 +2405,11 @@
       <c r="G46" t="b">
         <v>0</v>
       </c>
-      <c r="H46" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -2315,11 +2428,11 @@
       <c r="G47" t="b">
         <v>0</v>
       </c>
-      <c r="H47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -2338,11 +2451,11 @@
       <c r="G48" t="b">
         <v>0</v>
       </c>
-      <c r="H48" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -2361,11 +2474,11 @@
       <c r="G49" t="b">
         <v>0</v>
       </c>
-      <c r="H49" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -2384,11 +2497,11 @@
       <c r="G50" t="b">
         <v>0</v>
       </c>
-      <c r="H50" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -2407,11 +2520,11 @@
       <c r="G51" t="b">
         <v>0</v>
       </c>
-      <c r="H51" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -2430,11 +2543,11 @@
       <c r="G52" t="b">
         <v>0</v>
       </c>
-      <c r="H52" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -2453,11 +2566,11 @@
       <c r="G53" t="b">
         <v>0</v>
       </c>
-      <c r="H53" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2476,11 +2589,11 @@
       <c r="G54" t="b">
         <v>0</v>
       </c>
-      <c r="H54" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="I54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -2499,11 +2612,11 @@
       <c r="G55" t="b">
         <v>0</v>
       </c>
-      <c r="H55" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -2522,11 +2635,11 @@
       <c r="G56" t="b">
         <v>0</v>
       </c>
-      <c r="H56" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -2545,11 +2658,11 @@
       <c r="G57" t="b">
         <v>0</v>
       </c>
-      <c r="H57" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="I57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -2568,11 +2681,11 @@
       <c r="G58" t="b">
         <v>0</v>
       </c>
-      <c r="H58" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I58" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -2591,11 +2704,11 @@
       <c r="G59" t="b">
         <v>0</v>
       </c>
-      <c r="H59" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -2614,11 +2727,11 @@
       <c r="G60" t="b">
         <v>0</v>
       </c>
-      <c r="H60" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="I60" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>42</v>
       </c>
@@ -2637,11 +2750,11 @@
       <c r="G61" t="b">
         <v>0</v>
       </c>
-      <c r="H61" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="I61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -2660,11 +2773,11 @@
       <c r="G62" t="b">
         <v>0</v>
       </c>
-      <c r="H62" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="I62" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>42</v>
       </c>
@@ -2683,11 +2796,11 @@
       <c r="G63" t="b">
         <v>0</v>
       </c>
-      <c r="H63" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="I63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -2706,11 +2819,11 @@
       <c r="G64" t="b">
         <v>0</v>
       </c>
-      <c r="H64" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="I64" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -2729,11 +2842,11 @@
       <c r="G65" t="b">
         <v>0</v>
       </c>
-      <c r="H65" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="I65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -2752,11 +2865,11 @@
       <c r="G66" t="b">
         <v>0</v>
       </c>
-      <c r="H66" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="I66" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>42</v>
       </c>
@@ -2775,11 +2888,11 @@
       <c r="G67" t="b">
         <v>0</v>
       </c>
-      <c r="H67" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="I67" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>42</v>
       </c>
@@ -2798,11 +2911,11 @@
       <c r="G68" t="b">
         <v>0</v>
       </c>
-      <c r="H68" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="I68" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>42</v>
       </c>
@@ -2821,11 +2934,11 @@
       <c r="G69" t="b">
         <v>0</v>
       </c>
-      <c r="H69" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="I69" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>43</v>
       </c>
@@ -2844,11 +2957,11 @@
       <c r="G70" t="b">
         <v>0</v>
       </c>
-      <c r="H70" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I70" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>43</v>
       </c>
@@ -2867,11 +2980,11 @@
       <c r="G71" t="b">
         <v>0</v>
       </c>
-      <c r="H71" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="I71" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>43</v>
       </c>
@@ -2890,11 +3003,11 @@
       <c r="G72" t="b">
         <v>0</v>
       </c>
-      <c r="H72" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="I72" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>43</v>
       </c>
@@ -2913,11 +3026,11 @@
       <c r="G73" t="b">
         <v>0</v>
       </c>
-      <c r="H73" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="I73" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>43</v>
       </c>
@@ -2936,11 +3049,11 @@
       <c r="G74" t="b">
         <v>0</v>
       </c>
-      <c r="H74" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="I74" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>43</v>
       </c>
@@ -2959,11 +3072,11 @@
       <c r="G75" t="b">
         <v>0</v>
       </c>
-      <c r="H75" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="I75" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>43</v>
       </c>
@@ -2982,11 +3095,11 @@
       <c r="G76" t="b">
         <v>0</v>
       </c>
-      <c r="H76" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="I76" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>44</v>
       </c>
@@ -3005,11 +3118,11 @@
       <c r="G77" t="b">
         <v>0</v>
       </c>
-      <c r="H77" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="I77" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>44</v>
       </c>
@@ -3028,11 +3141,11 @@
       <c r="G78" t="b">
         <v>0</v>
       </c>
-      <c r="H78" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="I78" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>44</v>
       </c>
@@ -3051,11 +3164,11 @@
       <c r="G79" t="b">
         <v>0</v>
       </c>
-      <c r="H79" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="I79" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>44</v>
       </c>
@@ -3074,11 +3187,11 @@
       <c r="G80" t="b">
         <v>0</v>
       </c>
-      <c r="H80" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="I80" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>44</v>
       </c>
@@ -3097,11 +3210,11 @@
       <c r="G81" t="b">
         <v>0</v>
       </c>
-      <c r="H81" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="I81" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>44</v>
       </c>
@@ -3120,11 +3233,11 @@
       <c r="G82" t="b">
         <v>0</v>
       </c>
-      <c r="H82" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="I82" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -3143,11 +3256,11 @@
       <c r="G83" t="b">
         <v>0</v>
       </c>
-      <c r="H83" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="I83" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>44</v>
       </c>
@@ -3166,11 +3279,11 @@
       <c r="G84" t="b">
         <v>0</v>
       </c>
-      <c r="H84" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="I84" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>44</v>
       </c>
@@ -3189,11 +3302,11 @@
       <c r="G85" t="b">
         <v>0</v>
       </c>
-      <c r="H85" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="I85" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>44</v>
       </c>
@@ -3212,11 +3325,11 @@
       <c r="G86" t="b">
         <v>0</v>
       </c>
-      <c r="H86" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="I86" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>44</v>
       </c>
@@ -3235,11 +3348,11 @@
       <c r="G87" t="b">
         <v>0</v>
       </c>
-      <c r="H87" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="I87" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -3258,11 +3371,11 @@
       <c r="G88" t="b">
         <v>0</v>
       </c>
-      <c r="H88" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="I88" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -3281,11 +3394,11 @@
       <c r="G89" t="b">
         <v>0</v>
       </c>
-      <c r="H89" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="I89" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>44</v>
       </c>
@@ -3304,11 +3417,11 @@
       <c r="G90" t="b">
         <v>0</v>
       </c>
-      <c r="H90" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="I90" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>45</v>
       </c>
@@ -3327,11 +3440,11 @@
       <c r="G91" t="b">
         <v>0</v>
       </c>
-      <c r="H91" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="I91" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>45</v>
       </c>
@@ -3350,11 +3463,11 @@
       <c r="G92" t="b">
         <v>0</v>
       </c>
-      <c r="H92" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="I92" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>45</v>
       </c>
@@ -3373,11 +3486,11 @@
       <c r="G93" t="b">
         <v>0</v>
       </c>
-      <c r="H93" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="I93" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>45</v>
       </c>
@@ -3396,11 +3509,11 @@
       <c r="G94" t="b">
         <v>0</v>
       </c>
-      <c r="H94" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="I94" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>45</v>
       </c>
@@ -3419,11 +3532,11 @@
       <c r="G95" t="b">
         <v>0</v>
       </c>
-      <c r="H95" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="I95" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>45</v>
       </c>
@@ -3442,11 +3555,11 @@
       <c r="G96" t="b">
         <v>0</v>
       </c>
-      <c r="H96" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+      <c r="I96" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>45</v>
       </c>
@@ -3465,11 +3578,11 @@
       <c r="G97" t="b">
         <v>0</v>
       </c>
-      <c r="H97" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
+      <c r="I97" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>45</v>
       </c>
@@ -3488,11 +3601,11 @@
       <c r="G98" t="b">
         <v>0</v>
       </c>
-      <c r="H98" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="I98" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>45</v>
       </c>
@@ -3511,11 +3624,11 @@
       <c r="G99" t="b">
         <v>0</v>
       </c>
-      <c r="H99" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
+      <c r="I99" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>45</v>
       </c>
@@ -3534,11 +3647,11 @@
       <c r="G100" t="b">
         <v>0</v>
       </c>
-      <c r="H100" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+      <c r="I100" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>45</v>
       </c>
@@ -3557,11 +3670,11 @@
       <c r="G101" t="b">
         <v>0</v>
       </c>
-      <c r="H101" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
+      <c r="I101" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>45</v>
       </c>
@@ -3580,11 +3693,11 @@
       <c r="G102" t="b">
         <v>0</v>
       </c>
-      <c r="H102" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
+      <c r="I102" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>45</v>
       </c>
@@ -3603,11 +3716,11 @@
       <c r="G103" t="b">
         <v>0</v>
       </c>
-      <c r="H103" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
+      <c r="I103" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>46</v>
       </c>
@@ -3629,11 +3742,11 @@
       <c r="G104" t="b">
         <v>0</v>
       </c>
-      <c r="H104" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
+      <c r="I104" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>46</v>
       </c>
@@ -3655,11 +3768,11 @@
       <c r="G105" t="b">
         <v>0</v>
       </c>
-      <c r="H105" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
+      <c r="I105" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>46</v>
       </c>
@@ -3681,11 +3794,11 @@
       <c r="G106" t="b">
         <v>0</v>
       </c>
-      <c r="H106" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
+      <c r="I106" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -3707,11 +3820,11 @@
       <c r="G107" t="b">
         <v>0</v>
       </c>
-      <c r="H107" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
+      <c r="I107" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>46</v>
       </c>
@@ -3733,11 +3846,11 @@
       <c r="G108" t="b">
         <v>0</v>
       </c>
-      <c r="H108" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="I108" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>46</v>
       </c>
@@ -3759,11 +3872,11 @@
       <c r="G109" t="b">
         <v>0</v>
       </c>
-      <c r="H109" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
+      <c r="I109" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>46</v>
       </c>
@@ -3785,11 +3898,11 @@
       <c r="G110" t="b">
         <v>0</v>
       </c>
-      <c r="H110" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
+      <c r="I110" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>47</v>
       </c>
@@ -3808,11 +3921,11 @@
       <c r="G111" t="b">
         <v>0</v>
       </c>
-      <c r="H111" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
+      <c r="I111" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>47</v>
       </c>
@@ -3831,11 +3944,11 @@
       <c r="G112" t="b">
         <v>0</v>
       </c>
-      <c r="H112" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8">
+      <c r="I112" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
       <c r="A113" t="s">
         <v>47</v>
       </c>
@@ -3854,11 +3967,11 @@
       <c r="G113" t="b">
         <v>0</v>
       </c>
-      <c r="H113" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8">
+      <c r="I113" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
       <c r="A114" t="s">
         <v>47</v>
       </c>
@@ -3877,11 +3990,11 @@
       <c r="G114" t="b">
         <v>0</v>
       </c>
-      <c r="H114" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8">
+      <c r="I114" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115" t="s">
         <v>47</v>
       </c>
@@ -3900,11 +4013,11 @@
       <c r="G115" t="b">
         <v>0</v>
       </c>
-      <c r="H115" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
+      <c r="I115" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
       <c r="A116" t="s">
         <v>38</v>
       </c>
@@ -3926,11 +4039,14 @@
       <c r="G116" t="b">
         <v>1</v>
       </c>
-      <c r="H116" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="H116" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I116" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
       <c r="A117" t="s">
         <v>38</v>
       </c>
@@ -3952,11 +4068,14 @@
       <c r="G117" t="b">
         <v>0</v>
       </c>
-      <c r="H117" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8">
+      <c r="H117" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="I117" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
       <c r="A118" t="s">
         <v>38</v>
       </c>
@@ -3978,11 +4097,243 @@
       <c r="G118" t="b">
         <v>0</v>
       </c>
-      <c r="H118" t="s">
+      <c r="H118" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I118" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3" location="ProcessedData"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H116" r:id="rId6"/>
+    <hyperlink ref="H117" r:id="rId7"/>
+    <hyperlink ref="H118" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>160</v>
       </c>
+      <c r="B3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3" location="isAssociatedWith"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId6" location="isAssociatedWith"/>
+    <hyperlink ref="A4" r:id="rId7"/>
+    <hyperlink ref="C4" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId9" location="isAssociatedWith"/>
+    <hyperlink ref="A5" r:id="rId10"/>
+    <hyperlink ref="C5" r:id="rId11"/>
+    <hyperlink ref="F5" r:id="rId12" location="isAssociatedWith"/>
+    <hyperlink ref="A6" r:id="rId13"/>
+    <hyperlink ref="C6" r:id="rId14"/>
+    <hyperlink ref="F6" r:id="rId15" location="isAssociatedWith"/>
+    <hyperlink ref="A7" r:id="rId16"/>
+    <hyperlink ref="C7" r:id="rId17"/>
+    <hyperlink ref="F7" r:id="rId18" location="isAssociatedWith"/>
+    <hyperlink ref="A8" r:id="rId19"/>
+    <hyperlink ref="C8" r:id="rId20"/>
+    <hyperlink ref="F8" r:id="rId21" location="isAssociatedWith"/>
+    <hyperlink ref="A9" r:id="rId22" location="ProcessedData"/>
+    <hyperlink ref="C9" r:id="rId23" location="ProcessedData"/>
+    <hyperlink ref="F9" r:id="rId24" location="isAssociatedWith"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new columns; updated tags
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="193">
   <si>
     <t>cosasportal</t>
   </si>
@@ -25,7 +25,7 @@
     <t>COSAS Portal</t>
   </si>
   <si>
-    <t>Staging tables for raw data exports (v1.7.0, 2022-05-02)</t>
+    <t>Staging tables for raw data exports (v1.8.0, 2022-06-29)</t>
   </si>
   <si>
     <t>template</t>
@@ -364,6 +364,9 @@
     <t>CapturingKit</t>
   </si>
   <si>
+    <t>Project_Name</t>
+  </si>
+  <si>
     <t>GenomeBuild</t>
   </si>
   <si>
@@ -478,103 +481,100 @@
     <t>date the file was created</t>
   </si>
   <si>
+    <t>NCIT_C25364</t>
+  </si>
+  <si>
+    <t>SIO_001330</t>
+  </si>
+  <si>
+    <t>ProcessedData</t>
+  </si>
+  <si>
+    <t>NCIT_C164483</t>
+  </si>
+  <si>
+    <t>NCIT_C42628</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>compound</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>extends</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>idAttribute</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>nillable</t>
+  </si>
+  <si>
+    <t>lookupAttribute</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>dataType</t>
+  </si>
+  <si>
+    <t>defaultValue</t>
+  </si>
+  <si>
+    <t>partOfAttribute</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#ProcessedData</t>
+  </si>
+  <si>
     <t>http://semanticscience.org/resource/SIO_001330</t>
   </si>
   <si>
-    <t>https://w3id.org/reproduceme#ProcessedData</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>compound</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>package</t>
-  </si>
-  <si>
-    <t>abstract</t>
-  </si>
-  <si>
-    <t>extends</t>
-  </si>
-  <si>
-    <t>entity</t>
-  </si>
-  <si>
-    <t>idAttribute</t>
-  </si>
-  <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>nillable</t>
-  </si>
-  <si>
-    <t>lookupAttribute</t>
-  </si>
-  <si>
-    <t>tags</t>
-  </si>
-  <si>
-    <t>dataType</t>
-  </si>
-  <si>
-    <t>defaultValue</t>
-  </si>
-  <si>
-    <t>partOfAttribute</t>
-  </si>
-  <si>
-    <t>NCIT:C164483</t>
-  </si>
-  <si>
-    <t>NCIT:C25364</t>
-  </si>
-  <si>
-    <t>NCIT:C42628</t>
-  </si>
-  <si>
-    <t>SIO:001330</t>
-  </si>
-  <si>
-    <t>W3ID:ProcessedData</t>
-  </si>
-  <si>
     <t>NCIT</t>
   </si>
   <si>
     <t>SIO</t>
-  </si>
-  <si>
-    <t>W3ID</t>
   </si>
   <si>
     <t>isAssociatedWith</t>
@@ -963,13 +963,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -998,19 +998,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1154,7 +1154,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K120"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1162,37 +1162,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1203,7 +1203,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1217,11 +1217,11 @@
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>153</v>
+      <c r="H2" t="s">
+        <v>154</v>
       </c>
       <c r="I2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1232,7 +1232,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1246,11 +1246,11 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>154</v>
+      <c r="H3" t="s">
+        <v>155</v>
       </c>
       <c r="I3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1261,7 +1261,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1275,11 +1275,11 @@
       <c r="G4" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>155</v>
+      <c r="H4" t="s">
+        <v>156</v>
       </c>
       <c r="I4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -1293,7 +1293,7 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1307,11 +1307,11 @@
       <c r="G5" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>156</v>
+      <c r="H5" t="s">
+        <v>157</v>
       </c>
       <c r="I5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K5" t="s">
         <v>34</v>
@@ -1325,7 +1325,7 @@
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1339,11 +1339,11 @@
       <c r="G6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>157</v>
+      <c r="H6" t="s">
+        <v>158</v>
       </c>
       <c r="I6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K6" t="s">
         <v>34</v>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1415,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1438,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1530,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1576,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1599,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1668,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1691,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1760,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1783,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1829,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1898,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2013,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2036,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2082,7 +2082,7 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2128,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2151,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2266,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2381,7 +2381,7 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2404,7 +2404,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2427,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2519,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2542,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2565,7 +2565,7 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2611,7 +2611,7 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2634,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2680,7 +2680,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2703,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2795,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2818,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2841,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2910,7 +2910,7 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2933,7 +2933,7 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2956,7 +2956,7 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3025,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3048,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3094,7 +3094,7 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3117,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3140,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3186,7 +3186,7 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3209,7 +3209,7 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3255,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3301,7 +3301,7 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3324,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3370,7 +3370,7 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3393,7 +3393,7 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3439,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3462,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3508,7 +3508,7 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3531,7 +3531,7 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -3539,7 +3539,7 @@
         <v>30</v>
       </c>
       <c r="B102" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="D102" t="b">
         <v>0</v>
@@ -3554,7 +3554,7 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -3562,7 +3562,7 @@
         <v>30</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D103" t="b">
         <v>0</v>
@@ -3577,21 +3577,18 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B104" t="s">
-        <v>33</v>
-      </c>
-      <c r="C104" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="D104" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
@@ -3603,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -3611,13 +3608,13 @@
         <v>31</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="C105" t="s">
         <v>137</v>
       </c>
       <c r="D105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>
@@ -3629,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -3655,7 +3652,7 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -3681,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -3707,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -3733,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -3759,24 +3756,24 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B111" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="C111" t="s">
         <v>143</v>
       </c>
       <c r="D111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F111" t="b">
         <v>1</v>
@@ -3785,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -3793,16 +3790,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="C112" t="s">
         <v>144</v>
       </c>
       <c r="D112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112" t="b">
         <v>1</v>
@@ -3811,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -3837,7 +3834,7 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -3863,7 +3860,7 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -3889,7 +3886,7 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -3915,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -3941,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -3967,7 +3964,7 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -3993,7 +3990,7 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -4019,17 +4016,36 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
-        <v>158</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>32</v>
+      </c>
+      <c r="B121" t="s">
+        <v>131</v>
+      </c>
+      <c r="C121" t="s">
+        <v>153</v>
+      </c>
+      <c r="D121" t="b">
+        <v>0</v>
+      </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" t="b">
+        <v>1</v>
+      </c>
+      <c r="G121" t="b">
+        <v>0</v>
+      </c>
+      <c r="I121" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3" location="ProcessedData"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4047,7 +4063,7 @@
         <v>188</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>189</v>
@@ -4063,17 +4079,17 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>156</v>
+      <c r="A2" t="s">
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E2" t="s">
         <v>186</v>
@@ -4083,17 +4099,17 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>153</v>
+      <c r="A3" t="s">
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E3" t="s">
         <v>186</v>
@@ -4103,17 +4119,17 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>157</v>
+      <c r="A4" t="s">
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E4" t="s">
         <v>186</v>
@@ -4123,17 +4139,17 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>154</v>
+      <c r="A5" t="s">
+        <v>156</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
         <v>186</v>
@@ -4143,14 +4159,14 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="D6" t="s">
         <v>185</v>
@@ -4164,21 +4180,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3" location="isAssociatedWith"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6" location="isAssociatedWith"/>
-    <hyperlink ref="A4" r:id="rId7"/>
-    <hyperlink ref="C4" r:id="rId8"/>
-    <hyperlink ref="F4" r:id="rId9" location="isAssociatedWith"/>
-    <hyperlink ref="A5" r:id="rId10"/>
-    <hyperlink ref="C5" r:id="rId11"/>
-    <hyperlink ref="F5" r:id="rId12" location="isAssociatedWith"/>
-    <hyperlink ref="A6" r:id="rId13" location="ProcessedData"/>
-    <hyperlink ref="C6" r:id="rId14" location="ProcessedData"/>
-    <hyperlink ref="F6" r:id="rId15" location="isAssociatedWith"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2" location="isAssociatedWith"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4" location="isAssociatedWith"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="F4" r:id="rId6" location="isAssociatedWith"/>
+    <hyperlink ref="C5" r:id="rId7" location="ProcessedData"/>
+    <hyperlink ref="F5" r:id="rId8" location="isAssociatedWith"/>
+    <hyperlink ref="C6" r:id="rId9"/>
+    <hyperlink ref="F6" r:id="rId10" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new attributes to the portal
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="197">
   <si>
     <t>cosasportal</t>
   </si>
@@ -25,7 +25,7 @@
     <t>COSAS Portal</t>
   </si>
   <si>
-    <t>Staging tables for raw data exports (v1.8.0, 2022-06-29)</t>
+    <t>Staging tables for raw data exports (v1.9.0, 2022-07-21)</t>
   </si>
   <si>
     <t>template</t>
@@ -157,6 +157,15 @@
     <t>UMCG_VADER</t>
   </si>
   <si>
+    <t>FOETUS_ID</t>
+  </si>
+  <si>
+    <t>SAMPLEDATE</t>
+  </si>
+  <si>
+    <t>DISEASED</t>
+  </si>
+  <si>
     <t>HOOFDDIAGNOSE</t>
   </si>
   <si>
@@ -323,6 +332,9 @@
   </si>
   <si>
     <t>StandaardDeviatie</t>
+  </si>
+  <si>
+    <t>Foetus_Id</t>
   </si>
   <si>
     <t>GEN</t>
@@ -963,13 +975,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -998,19 +1010,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1154,7 +1166,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K121"/>
+  <dimension ref="A1:K129"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1162,37 +1174,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1203,7 +1215,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1218,10 +1230,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="I2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1232,7 +1244,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1247,10 +1259,10 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="I3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1261,7 +1273,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1276,10 +1288,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -1293,7 +1305,7 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1308,10 +1320,10 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="K5" t="s">
         <v>34</v>
@@ -1325,7 +1337,7 @@
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1340,10 +1352,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="K6" t="s">
         <v>34</v>
@@ -1369,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1392,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1415,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1438,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1461,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1484,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1507,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1530,15 +1542,15 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1553,15 +1565,15 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1576,15 +1588,15 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -1599,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1607,7 +1619,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1622,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1645,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1668,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1691,12 +1703,12 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
@@ -1714,12 +1726,12 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
@@ -1737,12 +1749,12 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
@@ -1760,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1783,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1806,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1852,7 +1864,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1875,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1898,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1921,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1944,7 +1956,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1967,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1990,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2036,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2059,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2082,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2105,7 +2117,7 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2128,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2151,15 +2163,15 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -2174,15 +2186,15 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -2197,15 +2209,15 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -2220,15 +2232,15 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -2243,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2251,7 +2263,7 @@
         <v>27</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2266,7 +2278,7 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2274,7 +2286,7 @@
         <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -2289,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2297,7 +2309,7 @@
         <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -2312,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2320,7 +2332,7 @@
         <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -2335,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2343,7 +2355,7 @@
         <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -2358,7 +2370,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2366,7 +2378,7 @@
         <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -2389,7 +2401,7 @@
         <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -2404,7 +2416,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2412,7 +2424,7 @@
         <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -2427,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2435,7 +2447,7 @@
         <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -2450,7 +2462,7 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2458,7 +2470,7 @@
         <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -2473,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2481,7 +2493,7 @@
         <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -2496,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2504,7 +2516,7 @@
         <v>27</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -2519,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2527,7 +2539,7 @@
         <v>27</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -2542,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2550,7 +2562,7 @@
         <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -2565,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2573,7 +2585,7 @@
         <v>27</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -2588,7 +2600,7 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2596,7 +2608,7 @@
         <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -2619,7 +2631,7 @@
         <v>27</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -2642,7 +2654,7 @@
         <v>27</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -2657,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2665,7 +2677,7 @@
         <v>27</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -2680,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2688,7 +2700,7 @@
         <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -2703,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2711,7 +2723,7 @@
         <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -2726,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2734,7 +2746,7 @@
         <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -2749,7 +2761,7 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2757,7 +2769,7 @@
         <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -2772,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2780,7 +2792,7 @@
         <v>27</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -2795,15 +2807,15 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -2818,15 +2830,15 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -2841,15 +2853,15 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -2864,15 +2876,15 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -2887,15 +2899,15 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -2910,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2918,7 +2930,7 @@
         <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -2933,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2941,7 +2953,7 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -2956,15 +2968,15 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -2979,15 +2991,15 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
@@ -3002,15 +3014,15 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="D79" t="b">
         <v>0</v>
@@ -3025,15 +3037,15 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
@@ -3048,15 +3060,15 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -3071,15 +3083,15 @@
         <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
@@ -3094,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3102,7 +3114,7 @@
         <v>29</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
@@ -3117,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3125,7 +3137,7 @@
         <v>29</v>
       </c>
       <c r="B84" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
@@ -3140,7 +3152,7 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3148,7 +3160,7 @@
         <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -3163,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3171,7 +3183,7 @@
         <v>29</v>
       </c>
       <c r="B86" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D86" t="b">
         <v>0</v>
@@ -3186,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3194,7 +3206,7 @@
         <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
@@ -3209,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3217,7 +3229,7 @@
         <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
@@ -3232,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3240,7 +3252,7 @@
         <v>29</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -3255,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3263,7 +3275,7 @@
         <v>29</v>
       </c>
       <c r="B90" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D90" t="b">
         <v>0</v>
@@ -3278,15 +3290,15 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
@@ -3301,15 +3313,15 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D92" t="b">
         <v>0</v>
@@ -3324,15 +3336,15 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D93" t="b">
         <v>0</v>
@@ -3347,15 +3359,15 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="D94" t="b">
         <v>0</v>
@@ -3370,15 +3382,15 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B95" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D95" t="b">
         <v>0</v>
@@ -3393,15 +3405,15 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B96" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D96" t="b">
         <v>0</v>
@@ -3416,15 +3428,15 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B97" t="s">
-        <v>112</v>
+        <v>46</v>
       </c>
       <c r="D97" t="b">
         <v>0</v>
@@ -3439,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3447,7 +3459,7 @@
         <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
@@ -3462,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3470,7 +3482,7 @@
         <v>30</v>
       </c>
       <c r="B99" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D99" t="b">
         <v>0</v>
@@ -3485,7 +3497,7 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3493,7 +3505,7 @@
         <v>30</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D100" t="b">
         <v>0</v>
@@ -3508,7 +3520,7 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3516,7 +3528,7 @@
         <v>30</v>
       </c>
       <c r="B101" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D101" t="b">
         <v>0</v>
@@ -3531,7 +3543,7 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -3539,7 +3551,7 @@
         <v>30</v>
       </c>
       <c r="B102" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D102" t="b">
         <v>0</v>
@@ -3554,7 +3566,7 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -3562,7 +3574,7 @@
         <v>30</v>
       </c>
       <c r="B103" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D103" t="b">
         <v>0</v>
@@ -3577,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -3585,7 +3597,7 @@
         <v>30</v>
       </c>
       <c r="B104" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -3600,21 +3612,18 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B105" t="s">
-        <v>33</v>
-      </c>
-      <c r="C105" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="D105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>
@@ -3626,18 +3635,15 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B106" t="s">
-        <v>117</v>
-      </c>
-      <c r="C106" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="D106" t="b">
         <v>0</v>
@@ -3652,18 +3658,15 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B107" t="s">
-        <v>118</v>
-      </c>
-      <c r="C107" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="D107" t="b">
         <v>0</v>
@@ -3678,19 +3681,16 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B108" t="s">
         <v>119</v>
       </c>
-      <c r="C108" t="s">
-        <v>140</v>
-      </c>
       <c r="D108" t="b">
         <v>0</v>
       </c>
@@ -3704,19 +3704,16 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B109" t="s">
         <v>120</v>
       </c>
-      <c r="C109" t="s">
-        <v>141</v>
-      </c>
       <c r="D109" t="b">
         <v>0</v>
       </c>
@@ -3730,18 +3727,15 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B110" t="s">
-        <v>121</v>
-      </c>
-      <c r="C110" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="D110" t="b">
         <v>0</v>
@@ -3756,18 +3750,15 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B111" t="s">
-        <v>122</v>
-      </c>
-      <c r="C111" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="D111" t="b">
         <v>0</v>
@@ -3787,19 +3778,16 @@
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B112" t="s">
-        <v>33</v>
-      </c>
-      <c r="C112" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="D112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F112" t="b">
         <v>1</v>
@@ -3808,21 +3796,21 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B113" t="s">
-        <v>123</v>
+        <v>33</v>
       </c>
       <c r="C113" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D113" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" t="b">
         <v>0</v>
@@ -3834,18 +3822,18 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B114" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C114" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D114" t="b">
         <v>0</v>
@@ -3860,18 +3848,18 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B115" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C115" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D115" t="b">
         <v>0</v>
@@ -3886,18 +3874,18 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B116" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C116" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D116" t="b">
         <v>0</v>
@@ -3912,18 +3900,18 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B117" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C117" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D117" t="b">
         <v>0</v>
@@ -3938,18 +3926,18 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C118" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D118" t="b">
         <v>0</v>
@@ -3964,18 +3952,18 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B119" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C119" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D119" t="b">
         <v>0</v>
@@ -3990,7 +3978,7 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -3998,16 +3986,16 @@
         <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="C120" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F120" t="b">
         <v>1</v>
@@ -4016,7 +4004,7 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -4024,25 +4012,233 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
+        <v>127</v>
+      </c>
+      <c r="C121" t="s">
+        <v>149</v>
+      </c>
+      <c r="D121" t="b">
+        <v>0</v>
+      </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" t="b">
+        <v>1</v>
+      </c>
+      <c r="G121" t="b">
+        <v>0</v>
+      </c>
+      <c r="I121" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>32</v>
+      </c>
+      <c r="B122" t="s">
+        <v>128</v>
+      </c>
+      <c r="C122" t="s">
+        <v>150</v>
+      </c>
+      <c r="D122" t="b">
+        <v>0</v>
+      </c>
+      <c r="E122" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122" t="b">
+        <v>1</v>
+      </c>
+      <c r="G122" t="b">
+        <v>0</v>
+      </c>
+      <c r="I122" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
+        <v>32</v>
+      </c>
+      <c r="B123" t="s">
+        <v>129</v>
+      </c>
+      <c r="C123" t="s">
+        <v>151</v>
+      </c>
+      <c r="D123" t="b">
+        <v>0</v>
+      </c>
+      <c r="E123" t="b">
+        <v>0</v>
+      </c>
+      <c r="F123" t="b">
+        <v>1</v>
+      </c>
+      <c r="G123" t="b">
+        <v>0</v>
+      </c>
+      <c r="I123" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" t="s">
+        <v>32</v>
+      </c>
+      <c r="B124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C124" t="s">
+        <v>152</v>
+      </c>
+      <c r="D124" t="b">
+        <v>0</v>
+      </c>
+      <c r="E124" t="b">
+        <v>0</v>
+      </c>
+      <c r="F124" t="b">
+        <v>1</v>
+      </c>
+      <c r="G124" t="b">
+        <v>0</v>
+      </c>
+      <c r="I124" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" t="s">
+        <v>32</v>
+      </c>
+      <c r="B125" t="s">
         <v>131</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C125" t="s">
         <v>153</v>
       </c>
-      <c r="D121" t="b">
-        <v>0</v>
-      </c>
-      <c r="E121" t="b">
-        <v>0</v>
-      </c>
-      <c r="F121" t="b">
-        <v>1</v>
-      </c>
-      <c r="G121" t="b">
-        <v>0</v>
-      </c>
-      <c r="I121" t="s">
-        <v>159</v>
+      <c r="D125" t="b">
+        <v>0</v>
+      </c>
+      <c r="E125" t="b">
+        <v>0</v>
+      </c>
+      <c r="F125" t="b">
+        <v>1</v>
+      </c>
+      <c r="G125" t="b">
+        <v>0</v>
+      </c>
+      <c r="I125" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B126" t="s">
+        <v>132</v>
+      </c>
+      <c r="C126" t="s">
+        <v>154</v>
+      </c>
+      <c r="D126" t="b">
+        <v>0</v>
+      </c>
+      <c r="E126" t="b">
+        <v>0</v>
+      </c>
+      <c r="F126" t="b">
+        <v>1</v>
+      </c>
+      <c r="G126" t="b">
+        <v>0</v>
+      </c>
+      <c r="I126" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" t="s">
+        <v>32</v>
+      </c>
+      <c r="B127" t="s">
+        <v>133</v>
+      </c>
+      <c r="C127" t="s">
+        <v>155</v>
+      </c>
+      <c r="D127" t="b">
+        <v>0</v>
+      </c>
+      <c r="E127" t="b">
+        <v>0</v>
+      </c>
+      <c r="F127" t="b">
+        <v>1</v>
+      </c>
+      <c r="G127" t="b">
+        <v>0</v>
+      </c>
+      <c r="I127" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" t="s">
+        <v>32</v>
+      </c>
+      <c r="B128" t="s">
+        <v>134</v>
+      </c>
+      <c r="C128" t="s">
+        <v>156</v>
+      </c>
+      <c r="D128" t="b">
+        <v>0</v>
+      </c>
+      <c r="E128" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128" t="b">
+        <v>1</v>
+      </c>
+      <c r="G128" t="b">
+        <v>0</v>
+      </c>
+      <c r="I128" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129" t="s">
+        <v>32</v>
+      </c>
+      <c r="B129" t="s">
+        <v>135</v>
+      </c>
+      <c r="C129" t="s">
+        <v>157</v>
+      </c>
+      <c r="D129" t="b">
+        <v>0</v>
+      </c>
+      <c r="E129" t="b">
+        <v>0</v>
+      </c>
+      <c r="F129" t="b">
+        <v>1</v>
+      </c>
+      <c r="G129" t="b">
+        <v>0</v>
+      </c>
+      <c r="I129" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -4060,122 +4256,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E4" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E6" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
init consent portal table
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="217">
   <si>
     <t>cosasportal</t>
   </si>
@@ -25,99 +25,108 @@
     <t>COSAS Portal</t>
   </si>
   <si>
-    <t>Staging tables for raw data exports (v1.9.0, 2022-07-21)</t>
+    <t>Staging tables for raw data exports (v2.0.0, 2022-11-09)</t>
   </si>
   <si>
     <t>template</t>
   </si>
   <si>
+    <t>cartagenia</t>
+  </si>
+  <si>
+    <t>consent</t>
+  </si>
+  <si>
+    <t>diagnoses</t>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>labs_array_adlas</t>
+  </si>
+  <si>
+    <t>labs_array_darwin</t>
+  </si>
+  <si>
+    <t>labs_ngs_adlas</t>
+  </si>
+  <si>
+    <t>labs_ngs_darwin</t>
+  </si>
+  <si>
     <t>patients</t>
   </si>
   <si>
-    <t>diagnoses</t>
-  </si>
-  <si>
     <t>samples</t>
   </si>
   <si>
-    <t>labs_array_adlas</t>
-  </si>
-  <si>
-    <t>labs_array_darwin</t>
-  </si>
-  <si>
-    <t>labs_ngs_adlas</t>
-  </si>
-  <si>
-    <t>labs_ngs_darwin</t>
-  </si>
-  <si>
-    <t>cartagenia</t>
-  </si>
-  <si>
-    <t>files</t>
-  </si>
-  <si>
     <t>attribute template for staging tables</t>
   </si>
   <si>
+    <t>Processed Cartagenia CNV bench data</t>
+  </si>
+  <si>
+    <t>Raw consent information open-exoom en 5PGM</t>
+  </si>
+  <si>
+    <t>Raw diagnostic metadata</t>
+  </si>
+  <si>
+    <t>Raw file metadata</t>
+  </si>
+  <si>
+    <t>Raw array metadata from ADLAS</t>
+  </si>
+  <si>
+    <t>Raw array metadata from Darwin</t>
+  </si>
+  <si>
+    <t>Raw NGS data from ADLAS</t>
+  </si>
+  <si>
+    <t>Raw NSG metadata from Darwin</t>
+  </si>
+  <si>
     <t>Raw metadata for patients and families</t>
   </si>
   <si>
-    <t>Raw diagnostic metadata</t>
-  </si>
-  <si>
     <t>Raw data table for samples</t>
   </si>
   <si>
-    <t>Raw array metadata from ADLAS</t>
-  </si>
-  <si>
-    <t>Raw array metadata from Darwin</t>
-  </si>
-  <si>
-    <t>Raw NGS data from ADLAS</t>
-  </si>
-  <si>
-    <t>Raw NSG metadata from Darwin</t>
-  </si>
-  <si>
-    <t>Processed Cartagenia CNV bench data</t>
-  </si>
-  <si>
-    <t>Raw file metadata</t>
-  </si>
-  <si>
     <t>cosasportal_template</t>
   </si>
   <si>
+    <t>cosasportal_cartagenia</t>
+  </si>
+  <si>
+    <t>cosasportal_consent</t>
+  </si>
+  <si>
+    <t>cosasportal_diagnoses</t>
+  </si>
+  <si>
+    <t>cosasportal_files</t>
+  </si>
+  <si>
+    <t>cosasportal_labs_array_adlas</t>
+  </si>
+  <si>
+    <t>cosasportal_labs_array_darwin</t>
+  </si>
+  <si>
+    <t>cosasportal_labs_ngs_adlas</t>
+  </si>
+  <si>
+    <t>cosasportal_labs_ngs_darwin</t>
+  </si>
+  <si>
     <t>cosasportal_patients</t>
   </si>
   <si>
-    <t>cosasportal_diagnoses</t>
-  </si>
-  <si>
     <t>cosasportal_samples</t>
   </si>
   <si>
-    <t>cosasportal_labs_array_adlas</t>
-  </si>
-  <si>
-    <t>cosasportal_labs_array_darwin</t>
-  </si>
-  <si>
-    <t>cosasportal_labs_ngs_adlas</t>
-  </si>
-  <si>
-    <t>cosasportal_labs_ngs_darwin</t>
-  </si>
-  <si>
-    <t>cosasportal_cartagenia</t>
-  </si>
-  <si>
-    <t>cosasportal_files</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -133,9 +142,276 @@
     <t>recordCreatedBy</t>
   </si>
   <si>
+    <t>subjectID</t>
+  </si>
+  <si>
+    <t>belongsToMother</t>
+  </si>
+  <si>
+    <t>belongsToFamily</t>
+  </si>
+  <si>
+    <t>isFetus</t>
+  </si>
+  <si>
+    <t>alternativeIdentifiers</t>
+  </si>
+  <si>
+    <t>observedPhenotype</t>
+  </si>
+  <si>
+    <t>analysis</t>
+  </si>
+  <si>
+    <t>datefilled</t>
+  </si>
+  <si>
+    <t>MDN_umcgnr</t>
+  </si>
+  <si>
+    <t>familienummer</t>
+  </si>
+  <si>
+    <t>request_consent_material</t>
+  </si>
+  <si>
+    <t>request_form</t>
+  </si>
+  <si>
+    <t>request_date_signed</t>
+  </si>
+  <si>
+    <t>consent_recontact</t>
+  </si>
+  <si>
+    <t>consent_research</t>
+  </si>
+  <si>
+    <t>consent_system</t>
+  </si>
+  <si>
+    <t>consent_form</t>
+  </si>
+  <si>
+    <t>consent_doctor</t>
+  </si>
+  <si>
+    <t>consent_date_signed</t>
+  </si>
+  <si>
+    <t>consent_folder</t>
+  </si>
+  <si>
+    <t>incidental_consent_recontact</t>
+  </si>
+  <si>
+    <t>incidental_form</t>
+  </si>
+  <si>
+    <t>incidental_date_signed</t>
+  </si>
+  <si>
     <t>UMCG_NUMBER</t>
   </si>
   <si>
+    <t>HOOFDDIAGNOSE</t>
+  </si>
+  <si>
+    <t>HOOFDDIAGNOSE_ZEKERHEID</t>
+  </si>
+  <si>
+    <t>EXTRA_DIAGNOSE</t>
+  </si>
+  <si>
+    <t>EXTRA_DIAGNOSE_ZEKERHEID</t>
+  </si>
+  <si>
+    <t>DATUM_EERSTE_CONSULT</t>
+  </si>
+  <si>
+    <t>OND_ID</t>
+  </si>
+  <si>
+    <t>umcgID</t>
+  </si>
+  <si>
+    <t>familyID</t>
+  </si>
+  <si>
+    <t>dnaID</t>
+  </si>
+  <si>
+    <t>testID</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>filepath</t>
+  </si>
+  <si>
+    <t>filetype</t>
+  </si>
+  <si>
+    <t>md5</t>
+  </si>
+  <si>
+    <t>dateCreated</t>
+  </si>
+  <si>
+    <t>ADVVRG_ID</t>
+  </si>
+  <si>
+    <t>DNA_NUMMER</t>
+  </si>
+  <si>
+    <t>TEST_ID</t>
+  </si>
+  <si>
+    <t>TEST_CODE</t>
+  </si>
+  <si>
+    <t>TEST_OMS</t>
+  </si>
+  <si>
+    <t>SGA_CHROMOSOME_REGION</t>
+  </si>
+  <si>
+    <t>SGA_CLASSIFICATION</t>
+  </si>
+  <si>
+    <t>SGA_CYTOBAND</t>
+  </si>
+  <si>
+    <t>SGA_DECIPHER_SYNDROMES</t>
+  </si>
+  <si>
+    <t>SGA_DGV_SIMILARITY</t>
+  </si>
+  <si>
+    <t>SGA_EVENT</t>
+  </si>
+  <si>
+    <t>SGA_EVIDENCE_SCORE</t>
+  </si>
+  <si>
+    <t>SGA_HMRELATED_GENES</t>
+  </si>
+  <si>
+    <t>SGA_HMRELATED_GENES_COUNT</t>
+  </si>
+  <si>
+    <t>SGA_LENGTH</t>
+  </si>
+  <si>
+    <t>SGA_MOSAIC</t>
+  </si>
+  <si>
+    <t>SGA_MOSAIC_PERCENTAGE</t>
+  </si>
+  <si>
+    <t>SGA_NO_OF_PROBES</t>
+  </si>
+  <si>
+    <t>SGA_NOTES</t>
+  </si>
+  <si>
+    <t>SGA_OMIM_MORBID_MAP</t>
+  </si>
+  <si>
+    <t>SGA_OMIM_MORBIDMAP_COUNT</t>
+  </si>
+  <si>
+    <t>SGA_PROBE_MEDIAN</t>
+  </si>
+  <si>
+    <t>SGA_REFSEQ_CODING_GENES</t>
+  </si>
+  <si>
+    <t>SGA_REFSEQ_CODING_GENES_COUNT</t>
+  </si>
+  <si>
+    <t>SGA_REGIONS_UMCG_CNV_NL_COUNT</t>
+  </si>
+  <si>
+    <t>SGA_SIMILAR_PREVIOUS_CASES</t>
+  </si>
+  <si>
+    <t>SGA_OVERERVING</t>
+  </si>
+  <si>
+    <t>FOETUS_ID</t>
+  </si>
+  <si>
+    <t>UmcgNr</t>
+  </si>
+  <si>
+    <t>TestId</t>
+  </si>
+  <si>
+    <t>TestDatum</t>
+  </si>
+  <si>
+    <t>Indicatie</t>
+  </si>
+  <si>
+    <t>BatchNaam</t>
+  </si>
+  <si>
+    <t>CallRate</t>
+  </si>
+  <si>
+    <t>StandaardDeviatie</t>
+  </si>
+  <si>
+    <t>Foetus_Id</t>
+  </si>
+  <si>
+    <t>GEN</t>
+  </si>
+  <si>
+    <t>MUTATIE</t>
+  </si>
+  <si>
+    <t>KLASSE</t>
+  </si>
+  <si>
+    <t>NM_NUMMER</t>
+  </si>
+  <si>
+    <t>LRGS_NUMMER</t>
+  </si>
+  <si>
+    <t>AMPLICON</t>
+  </si>
+  <si>
+    <t>ALLELFREQUENTIE</t>
+  </si>
+  <si>
+    <t>OVERERVING</t>
+  </si>
+  <si>
+    <t>Sequencer</t>
+  </si>
+  <si>
+    <t>PrepKit</t>
+  </si>
+  <si>
+    <t>SequencingType</t>
+  </si>
+  <si>
+    <t>SeqType</t>
+  </si>
+  <si>
+    <t>CapturingKit</t>
+  </si>
+  <si>
+    <t>Project_Name</t>
+  </si>
+  <si>
+    <t>GenomeBuild</t>
+  </si>
+  <si>
     <t>OVERLIJDENSDATUM</t>
   </si>
   <si>
@@ -157,54 +433,21 @@
     <t>UMCG_VADER</t>
   </si>
   <si>
-    <t>FOETUS_ID</t>
-  </si>
-  <si>
     <t>SAMPLEDATE</t>
   </si>
   <si>
     <t>DISEASED</t>
   </si>
   <si>
-    <t>HOOFDDIAGNOSE</t>
-  </si>
-  <si>
-    <t>HOOFDDIAGNOSE_ZEKERHEID</t>
-  </si>
-  <si>
-    <t>EXTRA_DIAGNOSE</t>
-  </si>
-  <si>
-    <t>EXTRA_DIAGNOSE_ZEKERHEID</t>
-  </si>
-  <si>
-    <t>DATUM_EERSTE_CONSULT</t>
-  </si>
-  <si>
-    <t>OND_ID</t>
-  </si>
-  <si>
     <t>UMCG_NUMMER</t>
   </si>
   <si>
-    <t>ADVVRG_ID</t>
-  </si>
-  <si>
     <t>ADVIESVRAAG_DATUM</t>
   </si>
   <si>
     <t>MONSTER_ID</t>
   </si>
   <si>
-    <t>TEST_CODE</t>
-  </si>
-  <si>
-    <t>TEST_OMS</t>
-  </si>
-  <si>
-    <t>DNA_NUMMER</t>
-  </si>
-  <si>
     <t>MATERIAAL</t>
   </si>
   <si>
@@ -244,189 +487,6 @@
     <t>AUTHORISED</t>
   </si>
   <si>
-    <t>TEST_ID</t>
-  </si>
-  <si>
-    <t>SGA_CHROMOSOME_REGION</t>
-  </si>
-  <si>
-    <t>SGA_CLASSIFICATION</t>
-  </si>
-  <si>
-    <t>SGA_CYTOBAND</t>
-  </si>
-  <si>
-    <t>SGA_DECIPHER_SYNDROMES</t>
-  </si>
-  <si>
-    <t>SGA_DGV_SIMILARITY</t>
-  </si>
-  <si>
-    <t>SGA_EVENT</t>
-  </si>
-  <si>
-    <t>SGA_EVIDENCE_SCORE</t>
-  </si>
-  <si>
-    <t>SGA_HMRELATED_GENES</t>
-  </si>
-  <si>
-    <t>SGA_HMRELATED_GENES_COUNT</t>
-  </si>
-  <si>
-    <t>SGA_LENGTH</t>
-  </si>
-  <si>
-    <t>SGA_MOSAIC</t>
-  </si>
-  <si>
-    <t>SGA_MOSAIC_PERCENTAGE</t>
-  </si>
-  <si>
-    <t>SGA_NO_OF_PROBES</t>
-  </si>
-  <si>
-    <t>SGA_NOTES</t>
-  </si>
-  <si>
-    <t>SGA_OMIM_MORBID_MAP</t>
-  </si>
-  <si>
-    <t>SGA_OMIM_MORBIDMAP_COUNT</t>
-  </si>
-  <si>
-    <t>SGA_PROBE_MEDIAN</t>
-  </si>
-  <si>
-    <t>SGA_REFSEQ_CODING_GENES</t>
-  </si>
-  <si>
-    <t>SGA_REFSEQ_CODING_GENES_COUNT</t>
-  </si>
-  <si>
-    <t>SGA_REGIONS_UMCG_CNV_NL_COUNT</t>
-  </si>
-  <si>
-    <t>SGA_SIMILAR_PREVIOUS_CASES</t>
-  </si>
-  <si>
-    <t>SGA_OVERERVING</t>
-  </si>
-  <si>
-    <t>UmcgNr</t>
-  </si>
-  <si>
-    <t>TestId</t>
-  </si>
-  <si>
-    <t>TestDatum</t>
-  </si>
-  <si>
-    <t>Indicatie</t>
-  </si>
-  <si>
-    <t>BatchNaam</t>
-  </si>
-  <si>
-    <t>CallRate</t>
-  </si>
-  <si>
-    <t>StandaardDeviatie</t>
-  </si>
-  <si>
-    <t>Foetus_Id</t>
-  </si>
-  <si>
-    <t>GEN</t>
-  </si>
-  <si>
-    <t>MUTATIE</t>
-  </si>
-  <si>
-    <t>KLASSE</t>
-  </si>
-  <si>
-    <t>NM_NUMMER</t>
-  </si>
-  <si>
-    <t>LRGS_NUMMER</t>
-  </si>
-  <si>
-    <t>AMPLICON</t>
-  </si>
-  <si>
-    <t>ALLELFREQUENTIE</t>
-  </si>
-  <si>
-    <t>OVERERVING</t>
-  </si>
-  <si>
-    <t>Sequencer</t>
-  </si>
-  <si>
-    <t>PrepKit</t>
-  </si>
-  <si>
-    <t>SequencingType</t>
-  </si>
-  <si>
-    <t>SeqType</t>
-  </si>
-  <si>
-    <t>CapturingKit</t>
-  </si>
-  <si>
-    <t>Project_Name</t>
-  </si>
-  <si>
-    <t>GenomeBuild</t>
-  </si>
-  <si>
-    <t>subjectID</t>
-  </si>
-  <si>
-    <t>belongsToMother</t>
-  </si>
-  <si>
-    <t>belongsToFamily</t>
-  </si>
-  <si>
-    <t>isFetus</t>
-  </si>
-  <si>
-    <t>alternativeIdentifiers</t>
-  </si>
-  <si>
-    <t>observedPhenotype</t>
-  </si>
-  <si>
-    <t>umcgID</t>
-  </si>
-  <si>
-    <t>familyID</t>
-  </si>
-  <si>
-    <t>dnaID</t>
-  </si>
-  <si>
-    <t>testID</t>
-  </si>
-  <si>
-    <t>filename</t>
-  </si>
-  <si>
-    <t>filepath</t>
-  </si>
-  <si>
-    <t>filetype</t>
-  </si>
-  <si>
-    <t>md5</t>
-  </si>
-  <si>
-    <t>dateCreated</t>
-  </si>
-  <si>
     <t>auto generated row identifier</t>
   </si>
   <si>
@@ -568,19 +628,19 @@
     <t>partOfAttribute</t>
   </si>
   <si>
+    <t>ProcessedData https://w3id.org/reproduceme#ProcessedData</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001330</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
-  </si>
-  <si>
-    <t>https://w3id.org/reproduceme#ProcessedData</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001330</t>
   </si>
   <si>
     <t>NCIT</t>
@@ -975,13 +1035,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1002,7 +1062,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1010,19 +1070,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1033,7 +1093,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1047,10 +1107,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1061,10 +1118,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1075,10 +1129,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1089,10 +1143,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1103,10 +1154,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1117,10 +1168,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1131,10 +1182,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1145,7 +1196,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1156,7 +1210,24 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1166,7 +1237,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:K147"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1174,48 +1245,48 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1230,21 +1301,21 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="I2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1259,21 +1330,21 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="I3" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1288,10 +1359,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="I4" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -1299,13 +1370,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1320,56 +1391,59 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="I5" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>182</v>
+      </c>
+      <c r="I6" t="s">
+        <v>183</v>
+      </c>
+      <c r="K6" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>162</v>
-      </c>
-      <c r="I6" t="s">
-        <v>163</v>
-      </c>
-      <c r="K6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>161</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1381,15 +1455,18 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>162</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1404,15 +1481,18 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>163</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -1427,15 +1507,18 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>164</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -1450,15 +1533,18 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>165</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1473,15 +1559,18 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>166</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1496,15 +1585,18 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>167</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1519,15 +1611,15 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1542,15 +1634,15 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1565,15 +1657,15 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1588,15 +1680,15 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -1611,15 +1703,15 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1634,15 +1726,15 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -1657,15 +1749,15 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1680,15 +1772,15 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -1703,15 +1795,15 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1726,15 +1818,15 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -1749,15 +1841,15 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -1772,15 +1864,15 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -1795,15 +1887,15 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -1818,15 +1910,15 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -1841,15 +1933,15 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1864,15 +1956,15 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -1887,15 +1979,15 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -1910,38 +2002,38 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="D31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -1956,15 +2048,15 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -1979,15 +2071,15 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -2002,15 +2094,15 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -2025,15 +2117,15 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -2048,15 +2140,15 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -2071,15 +2163,15 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -2094,21 +2186,24 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>168</v>
       </c>
       <c r="D39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -2117,15 +2212,18 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="C40" t="s">
+        <v>169</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -2140,15 +2238,18 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="C41" t="s">
+        <v>170</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -2163,15 +2264,18 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="C42" t="s">
+        <v>171</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -2186,15 +2290,18 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
+        <v>172</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -2209,15 +2316,18 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="C44" t="s">
+        <v>173</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -2232,15 +2342,18 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
+        <v>174</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -2255,15 +2368,18 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>77</v>
+      </c>
+      <c r="C46" t="s">
+        <v>175</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2278,15 +2394,18 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>78</v>
+      </c>
+      <c r="C47" t="s">
+        <v>176</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -2301,15 +2420,18 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
+        <v>177</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -2324,15 +2446,15 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -2347,15 +2469,15 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -2370,15 +2492,15 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -2393,15 +2515,15 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -2416,15 +2538,15 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -2439,15 +2561,15 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -2462,15 +2584,15 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -2485,15 +2607,15 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -2508,15 +2630,15 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -2531,15 +2653,15 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -2554,15 +2676,15 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -2577,15 +2699,15 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -2600,15 +2722,15 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -2623,15 +2745,15 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -2646,15 +2768,15 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -2669,15 +2791,15 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B64" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -2692,15 +2814,15 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -2715,15 +2837,15 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -2738,15 +2860,15 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -2761,15 +2883,15 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -2784,15 +2906,15 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B69" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -2807,15 +2929,15 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -2830,15 +2952,15 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -2853,15 +2975,15 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -2876,15 +2998,15 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B73" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -2899,15 +3021,15 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -2922,15 +3044,15 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B75" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -2945,15 +3067,15 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B76" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -2968,15 +3090,15 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B77" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -2991,15 +3113,15 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
@@ -3014,15 +3136,15 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D79" t="b">
         <v>0</v>
@@ -3037,15 +3159,15 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B80" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
@@ -3060,15 +3182,15 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B81" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -3083,15 +3205,15 @@
         <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B82" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
@@ -3106,15 +3228,15 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
@@ -3129,15 +3251,15 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
@@ -3152,15 +3274,15 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B85" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -3175,15 +3297,15 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D86" t="b">
         <v>0</v>
@@ -3198,15 +3320,15 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
@@ -3221,15 +3343,15 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
@@ -3244,15 +3366,15 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -3267,15 +3389,15 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D90" t="b">
         <v>0</v>
@@ -3290,15 +3412,15 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
@@ -3313,15 +3435,15 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D92" t="b">
         <v>0</v>
@@ -3336,15 +3458,15 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D93" t="b">
         <v>0</v>
@@ -3359,15 +3481,15 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="D94" t="b">
         <v>0</v>
@@ -3382,15 +3504,15 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D95" t="b">
         <v>0</v>
@@ -3405,15 +3527,15 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D96" t="b">
         <v>0</v>
@@ -3428,15 +3550,15 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="D97" t="b">
         <v>0</v>
@@ -3451,15 +3573,15 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
@@ -3474,15 +3596,15 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="D99" t="b">
         <v>0</v>
@@ -3497,15 +3619,15 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D100" t="b">
         <v>0</v>
@@ -3520,15 +3642,15 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D101" t="b">
         <v>0</v>
@@ -3543,15 +3665,15 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B102" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D102" t="b">
         <v>0</v>
@@ -3566,15 +3688,15 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D103" t="b">
         <v>0</v>
@@ -3589,15 +3711,15 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -3612,15 +3734,15 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D105" t="b">
         <v>0</v>
@@ -3635,15 +3757,15 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D106" t="b">
         <v>0</v>
@@ -3658,15 +3780,15 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B107" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="D107" t="b">
         <v>0</v>
@@ -3681,15 +3803,15 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B108" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D108" t="b">
         <v>0</v>
@@ -3704,15 +3826,15 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D109" t="b">
         <v>0</v>
@@ -3727,15 +3849,15 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D110" t="b">
         <v>0</v>
@@ -3750,15 +3872,15 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B111" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="D111" t="b">
         <v>0</v>
@@ -3773,15 +3895,15 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B112" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="D112" t="b">
         <v>0</v>
@@ -3796,21 +3918,18 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B113" t="s">
-        <v>33</v>
-      </c>
-      <c r="C113" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="D113" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E113" t="b">
         <v>0</v>
@@ -3822,18 +3941,15 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B114" t="s">
-        <v>121</v>
-      </c>
-      <c r="C114" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="D114" t="b">
         <v>0</v>
@@ -3848,18 +3964,15 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B115" t="s">
-        <v>122</v>
-      </c>
-      <c r="C115" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="D115" t="b">
         <v>0</v>
@@ -3874,18 +3987,15 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B116" t="s">
-        <v>123</v>
-      </c>
-      <c r="C116" t="s">
-        <v>144</v>
+        <v>64</v>
       </c>
       <c r="D116" t="b">
         <v>0</v>
@@ -3900,18 +4010,15 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B117" t="s">
-        <v>124</v>
-      </c>
-      <c r="C117" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="D117" t="b">
         <v>0</v>
@@ -3926,18 +4033,15 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B118" t="s">
-        <v>125</v>
-      </c>
-      <c r="C118" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D118" t="b">
         <v>0</v>
@@ -3952,18 +4056,15 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C119" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="D119" t="b">
         <v>0</v>
@@ -3978,24 +4079,21 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B120" t="s">
-        <v>33</v>
-      </c>
-      <c r="C120" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="D120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F120" t="b">
         <v>1</v>
@@ -4004,18 +4102,15 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B121" t="s">
-        <v>127</v>
-      </c>
-      <c r="C121" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D121" t="b">
         <v>0</v>
@@ -4030,18 +4125,15 @@
         <v>0</v>
       </c>
       <c r="I121" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B122" t="s">
-        <v>128</v>
-      </c>
-      <c r="C122" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D122" t="b">
         <v>0</v>
@@ -4056,18 +4148,15 @@
         <v>0</v>
       </c>
       <c r="I122" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B123" t="s">
-        <v>129</v>
-      </c>
-      <c r="C123" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="D123" t="b">
         <v>0</v>
@@ -4082,18 +4171,15 @@
         <v>0</v>
       </c>
       <c r="I123" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B124" t="s">
-        <v>130</v>
-      </c>
-      <c r="C124" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="D124" t="b">
         <v>0</v>
@@ -4108,18 +4194,15 @@
         <v>0</v>
       </c>
       <c r="I124" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B125" t="s">
-        <v>131</v>
-      </c>
-      <c r="C125" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D125" t="b">
         <v>0</v>
@@ -4134,18 +4217,15 @@
         <v>0</v>
       </c>
       <c r="I125" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B126" t="s">
-        <v>132</v>
-      </c>
-      <c r="C126" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="D126" t="b">
         <v>0</v>
@@ -4160,18 +4240,15 @@
         <v>0</v>
       </c>
       <c r="I126" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B127" t="s">
-        <v>133</v>
-      </c>
-      <c r="C127" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D127" t="b">
         <v>0</v>
@@ -4186,18 +4263,15 @@
         <v>0</v>
       </c>
       <c r="I127" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B128" t="s">
-        <v>134</v>
-      </c>
-      <c r="C128" t="s">
-        <v>156</v>
+        <v>80</v>
       </c>
       <c r="D128" t="b">
         <v>0</v>
@@ -4212,18 +4286,15 @@
         <v>0</v>
       </c>
       <c r="I128" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B129" t="s">
-        <v>135</v>
-      </c>
-      <c r="C129" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D129" t="b">
         <v>0</v>
@@ -4238,7 +4309,421 @@
         <v>0</v>
       </c>
       <c r="I129" t="s">
-        <v>163</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130" t="s">
+        <v>35</v>
+      </c>
+      <c r="B130" t="s">
+        <v>142</v>
+      </c>
+      <c r="D130" t="b">
+        <v>0</v>
+      </c>
+      <c r="E130" t="b">
+        <v>0</v>
+      </c>
+      <c r="F130" t="b">
+        <v>1</v>
+      </c>
+      <c r="G130" t="b">
+        <v>0</v>
+      </c>
+      <c r="I130" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" t="s">
+        <v>35</v>
+      </c>
+      <c r="B131" t="s">
+        <v>83</v>
+      </c>
+      <c r="D131" t="b">
+        <v>0</v>
+      </c>
+      <c r="E131" t="b">
+        <v>0</v>
+      </c>
+      <c r="F131" t="b">
+        <v>1</v>
+      </c>
+      <c r="G131" t="b">
+        <v>0</v>
+      </c>
+      <c r="I131" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" t="s">
+        <v>35</v>
+      </c>
+      <c r="B132" t="s">
+        <v>84</v>
+      </c>
+      <c r="D132" t="b">
+        <v>0</v>
+      </c>
+      <c r="E132" t="b">
+        <v>0</v>
+      </c>
+      <c r="F132" t="b">
+        <v>1</v>
+      </c>
+      <c r="G132" t="b">
+        <v>0</v>
+      </c>
+      <c r="I132" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" t="s">
+        <v>35</v>
+      </c>
+      <c r="B133" t="s">
+        <v>81</v>
+      </c>
+      <c r="D133" t="b">
+        <v>0</v>
+      </c>
+      <c r="E133" t="b">
+        <v>0</v>
+      </c>
+      <c r="F133" t="b">
+        <v>1</v>
+      </c>
+      <c r="G133" t="b">
+        <v>0</v>
+      </c>
+      <c r="I133" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" t="s">
+        <v>35</v>
+      </c>
+      <c r="B134" t="s">
+        <v>143</v>
+      </c>
+      <c r="D134" t="b">
+        <v>0</v>
+      </c>
+      <c r="E134" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134" t="b">
+        <v>1</v>
+      </c>
+      <c r="G134" t="b">
+        <v>0</v>
+      </c>
+      <c r="I134" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135" t="s">
+        <v>35</v>
+      </c>
+      <c r="B135" t="s">
+        <v>144</v>
+      </c>
+      <c r="D135" t="b">
+        <v>0</v>
+      </c>
+      <c r="E135" t="b">
+        <v>0</v>
+      </c>
+      <c r="F135" t="b">
+        <v>1</v>
+      </c>
+      <c r="G135" t="b">
+        <v>0</v>
+      </c>
+      <c r="I135" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" t="s">
+        <v>35</v>
+      </c>
+      <c r="B136" t="s">
+        <v>145</v>
+      </c>
+      <c r="D136" t="b">
+        <v>0</v>
+      </c>
+      <c r="E136" t="b">
+        <v>0</v>
+      </c>
+      <c r="F136" t="b">
+        <v>1</v>
+      </c>
+      <c r="G136" t="b">
+        <v>0</v>
+      </c>
+      <c r="I136" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="A137" t="s">
+        <v>35</v>
+      </c>
+      <c r="B137" t="s">
+        <v>146</v>
+      </c>
+      <c r="D137" t="b">
+        <v>0</v>
+      </c>
+      <c r="E137" t="b">
+        <v>0</v>
+      </c>
+      <c r="F137" t="b">
+        <v>1</v>
+      </c>
+      <c r="G137" t="b">
+        <v>0</v>
+      </c>
+      <c r="I137" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="A138" t="s">
+        <v>35</v>
+      </c>
+      <c r="B138" t="s">
+        <v>147</v>
+      </c>
+      <c r="D138" t="b">
+        <v>0</v>
+      </c>
+      <c r="E138" t="b">
+        <v>0</v>
+      </c>
+      <c r="F138" t="b">
+        <v>1</v>
+      </c>
+      <c r="G138" t="b">
+        <v>0</v>
+      </c>
+      <c r="I138" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="A139" t="s">
+        <v>35</v>
+      </c>
+      <c r="B139" t="s">
+        <v>148</v>
+      </c>
+      <c r="D139" t="b">
+        <v>0</v>
+      </c>
+      <c r="E139" t="b">
+        <v>0</v>
+      </c>
+      <c r="F139" t="b">
+        <v>1</v>
+      </c>
+      <c r="G139" t="b">
+        <v>0</v>
+      </c>
+      <c r="I139" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="A140" t="s">
+        <v>35</v>
+      </c>
+      <c r="B140" t="s">
+        <v>149</v>
+      </c>
+      <c r="D140" t="b">
+        <v>0</v>
+      </c>
+      <c r="E140" t="b">
+        <v>0</v>
+      </c>
+      <c r="F140" t="b">
+        <v>1</v>
+      </c>
+      <c r="G140" t="b">
+        <v>0</v>
+      </c>
+      <c r="I140" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" t="s">
+        <v>35</v>
+      </c>
+      <c r="B141" t="s">
+        <v>150</v>
+      </c>
+      <c r="D141" t="b">
+        <v>0</v>
+      </c>
+      <c r="E141" t="b">
+        <v>0</v>
+      </c>
+      <c r="F141" t="b">
+        <v>1</v>
+      </c>
+      <c r="G141" t="b">
+        <v>0</v>
+      </c>
+      <c r="I141" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="A142" t="s">
+        <v>35</v>
+      </c>
+      <c r="B142" t="s">
+        <v>151</v>
+      </c>
+      <c r="D142" t="b">
+        <v>0</v>
+      </c>
+      <c r="E142" t="b">
+        <v>0</v>
+      </c>
+      <c r="F142" t="b">
+        <v>1</v>
+      </c>
+      <c r="G142" t="b">
+        <v>0</v>
+      </c>
+      <c r="I142" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143" t="s">
+        <v>35</v>
+      </c>
+      <c r="B143" t="s">
+        <v>152</v>
+      </c>
+      <c r="D143" t="b">
+        <v>0</v>
+      </c>
+      <c r="E143" t="b">
+        <v>0</v>
+      </c>
+      <c r="F143" t="b">
+        <v>1</v>
+      </c>
+      <c r="G143" t="b">
+        <v>0</v>
+      </c>
+      <c r="I143" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="A144" t="s">
+        <v>35</v>
+      </c>
+      <c r="B144" t="s">
+        <v>153</v>
+      </c>
+      <c r="D144" t="b">
+        <v>0</v>
+      </c>
+      <c r="E144" t="b">
+        <v>0</v>
+      </c>
+      <c r="F144" t="b">
+        <v>1</v>
+      </c>
+      <c r="G144" t="b">
+        <v>0</v>
+      </c>
+      <c r="I144" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
+      <c r="A145" t="s">
+        <v>35</v>
+      </c>
+      <c r="B145" t="s">
+        <v>154</v>
+      </c>
+      <c r="D145" t="b">
+        <v>0</v>
+      </c>
+      <c r="E145" t="b">
+        <v>0</v>
+      </c>
+      <c r="F145" t="b">
+        <v>1</v>
+      </c>
+      <c r="G145" t="b">
+        <v>0</v>
+      </c>
+      <c r="I145" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" t="s">
+        <v>35</v>
+      </c>
+      <c r="B146" t="s">
+        <v>155</v>
+      </c>
+      <c r="D146" t="b">
+        <v>0</v>
+      </c>
+      <c r="E146" t="b">
+        <v>0</v>
+      </c>
+      <c r="F146" t="b">
+        <v>1</v>
+      </c>
+      <c r="G146" t="b">
+        <v>0</v>
+      </c>
+      <c r="I146" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" t="s">
+        <v>35</v>
+      </c>
+      <c r="B147" t="s">
+        <v>107</v>
+      </c>
+      <c r="D147" t="b">
+        <v>0</v>
+      </c>
+      <c r="E147" t="b">
+        <v>0</v>
+      </c>
+      <c r="F147" t="b">
+        <v>1</v>
+      </c>
+      <c r="G147" t="b">
+        <v>0</v>
+      </c>
+      <c r="I147" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4256,136 +4741,129 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D3" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="E5" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="E6" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="F2" r:id="rId2" location="isAssociatedWith"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4" location="isAssociatedWith"/>
-    <hyperlink ref="C4" r:id="rId5"/>
-    <hyperlink ref="F4" r:id="rId6" location="isAssociatedWith"/>
-    <hyperlink ref="C5" r:id="rId7" location="ProcessedData"/>
-    <hyperlink ref="F5" r:id="rId8" location="isAssociatedWith"/>
-    <hyperlink ref="C6" r:id="rId9"/>
-    <hyperlink ref="F6" r:id="rId10" location="isAssociatedWith"/>
+    <hyperlink ref="F3" r:id="rId3" location="isAssociatedWith"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5" location="isAssociatedWith"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="F5" r:id="rId7" location="isAssociatedWith"/>
+    <hyperlink ref="C6" r:id="rId8"/>
+    <hyperlink ref="F6" r:id="rId9" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: added missing attribute
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="235">
   <si>
     <t>cosasportal</t>
   </si>
@@ -25,7 +25,7 @@
     <t>COSAS Portal</t>
   </si>
   <si>
-    <t>Staging tables for raw data exports (v2.1.0, 2023-07-24)</t>
+    <t>Staging tables for raw data exports (v2.1.1, 2023-07-25)</t>
   </si>
   <si>
     <t>template</t>
@@ -187,6 +187,9 @@
     <t>request_date_signed</t>
   </si>
   <si>
+    <t>consent_diagnostics</t>
+  </si>
+  <si>
     <t>consent_recontact</t>
   </si>
   <si>
@@ -682,16 +685,16 @@
     <t>ProcessedData https://w3id.org/reproduceme#ProcessedData</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001330</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001330</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
   </si>
   <si>
     <t>NCIT</t>
@@ -1086,13 +1089,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1121,19 +1124,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1296,7 +1299,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K162"/>
+  <dimension ref="A1:K163"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1304,37 +1307,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1345,7 +1348,7 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1360,10 +1363,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1374,7 +1377,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1389,10 +1392,10 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1403,7 +1406,7 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1418,10 +1421,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -1435,7 +1438,7 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1450,10 +1453,10 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K5" t="s">
         <v>39</v>
@@ -1467,7 +1470,7 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1482,10 +1485,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K6" t="s">
         <v>39</v>
@@ -1499,7 +1502,7 @@
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -1514,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1525,7 +1528,7 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1540,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1551,7 +1554,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -1566,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1577,7 +1580,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -1592,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1603,7 +1606,7 @@
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1618,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1629,7 +1632,7 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1644,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1655,7 +1658,7 @@
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1670,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1693,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1716,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1739,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1762,7 +1765,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1785,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1808,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1831,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1854,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1877,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1900,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1923,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1946,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1969,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1992,7 +1995,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2015,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2038,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2061,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2069,45 +2072,45 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="D31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="D32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2130,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2153,7 +2156,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2176,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2199,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2222,7 +2225,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2245,12 +2248,12 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
         <v>73</v>
@@ -2268,7 +2271,7 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2291,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2314,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2337,7 +2340,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2360,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2383,7 +2386,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2406,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2414,7 +2417,7 @@
         <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2429,7 +2432,7 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2437,7 +2440,7 @@
         <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -2452,7 +2455,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2475,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2498,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2521,7 +2524,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2532,10 +2535,10 @@
         <v>84</v>
       </c>
       <c r="D51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
@@ -2544,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2555,7 +2558,7 @@
         <v>85</v>
       </c>
       <c r="D52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -2567,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2581,7 +2584,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="b">
         <v>1</v>
@@ -2590,27 +2593,21 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>201</v>
-      </c>
-      <c r="J53" t="b">
-        <v>0</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
-      </c>
-      <c r="C54" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
       <c r="D54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" t="b">
         <v>1</v>
@@ -2619,7 +2616,10 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>199</v>
+        <v>202</v>
+      </c>
+      <c r="J54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2627,16 +2627,16 @@
         <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="C55" t="s">
         <v>185</v>
       </c>
       <c r="D55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -2645,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2671,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2723,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2775,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2853,15 +2853,18 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>96</v>
+      </c>
+      <c r="C64" t="s">
+        <v>194</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -2876,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2884,7 +2887,7 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -2899,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2922,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2945,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2968,7 +2971,7 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2991,7 +2994,7 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3014,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -3037,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3060,7 +3063,7 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3083,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3106,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3129,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3152,7 +3155,7 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3175,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3198,7 +3201,7 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3221,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3244,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3267,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3290,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3313,7 +3316,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3336,7 +3339,7 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3359,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3382,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3405,7 +3408,7 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3428,7 +3431,7 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3451,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3474,7 +3477,7 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3497,7 +3500,7 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3520,12 +3523,12 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B93" t="s">
         <v>124</v>
@@ -3543,7 +3546,7 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3566,7 +3569,7 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3589,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3612,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3635,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3658,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3681,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3704,15 +3707,15 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B101" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="D101" t="b">
         <v>0</v>
@@ -3727,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -3735,7 +3738,7 @@
         <v>34</v>
       </c>
       <c r="B102" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="D102" t="b">
         <v>0</v>
@@ -3750,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -3773,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -3796,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -3819,7 +3822,7 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -3842,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -3850,7 +3853,7 @@
         <v>34</v>
       </c>
       <c r="B107" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="D107" t="b">
         <v>0</v>
@@ -3865,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -3888,7 +3891,7 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -3911,7 +3914,7 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -3934,7 +3937,7 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -3957,7 +3960,7 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -3980,7 +3983,7 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -4003,7 +4006,7 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4026,7 +4029,7 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -4034,7 +4037,7 @@
         <v>34</v>
       </c>
       <c r="B115" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="D115" t="b">
         <v>0</v>
@@ -4049,12 +4052,12 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B116" t="s">
         <v>124</v>
@@ -4072,7 +4075,7 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -4095,7 +4098,7 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -4118,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -4141,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -4149,7 +4152,7 @@
         <v>35</v>
       </c>
       <c r="B120" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D120" t="b">
         <v>0</v>
@@ -4164,7 +4167,7 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -4187,7 +4190,7 @@
         <v>0</v>
       </c>
       <c r="I121" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -4210,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="I122" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -4233,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="I123" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -4256,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="I124" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -4264,7 +4267,7 @@
         <v>35</v>
       </c>
       <c r="B125" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="D125" t="b">
         <v>0</v>
@@ -4279,7 +4282,7 @@
         <v>0</v>
       </c>
       <c r="I125" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -4287,7 +4290,7 @@
         <v>35</v>
       </c>
       <c r="B126" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D126" t="b">
         <v>0</v>
@@ -4302,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="I126" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4325,7 +4328,7 @@
         <v>0</v>
       </c>
       <c r="I127" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -4333,7 +4336,7 @@
         <v>35</v>
       </c>
       <c r="B128" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="D128" t="b">
         <v>0</v>
@@ -4348,7 +4351,7 @@
         <v>0</v>
       </c>
       <c r="I128" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -4371,7 +4374,7 @@
         <v>0</v>
       </c>
       <c r="I129" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4394,15 +4397,15 @@
         <v>0</v>
       </c>
       <c r="I130" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="131" spans="1:9">
       <c r="A131" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B131" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="D131" t="b">
         <v>0</v>
@@ -4417,7 +4420,7 @@
         <v>0</v>
       </c>
       <c r="I131" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -4425,7 +4428,7 @@
         <v>36</v>
       </c>
       <c r="B132" t="s">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="D132" t="b">
         <v>0</v>
@@ -4440,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="I132" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -4463,7 +4466,7 @@
         <v>0</v>
       </c>
       <c r="I133" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -4486,7 +4489,7 @@
         <v>0</v>
       </c>
       <c r="I134" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4509,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="I135" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -4532,7 +4535,7 @@
         <v>0</v>
       </c>
       <c r="I136" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -4555,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="I137" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4578,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="I138" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4586,7 +4589,7 @@
         <v>36</v>
       </c>
       <c r="B139" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="D139" t="b">
         <v>0</v>
@@ -4601,7 +4604,7 @@
         <v>0</v>
       </c>
       <c r="I139" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -4609,7 +4612,7 @@
         <v>36</v>
       </c>
       <c r="B140" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="D140" t="b">
         <v>0</v>
@@ -4624,7 +4627,7 @@
         <v>0</v>
       </c>
       <c r="I140" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -4647,12 +4650,12 @@
         <v>0</v>
       </c>
       <c r="I141" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B142" t="s">
         <v>156</v>
@@ -4670,7 +4673,7 @@
         <v>0</v>
       </c>
       <c r="I142" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -4678,7 +4681,7 @@
         <v>37</v>
       </c>
       <c r="B143" t="s">
-        <v>96</v>
+        <v>157</v>
       </c>
       <c r="D143" t="b">
         <v>0</v>
@@ -4693,7 +4696,7 @@
         <v>0</v>
       </c>
       <c r="I143" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -4701,7 +4704,7 @@
         <v>37</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="D144" t="b">
         <v>0</v>
@@ -4716,7 +4719,7 @@
         <v>0</v>
       </c>
       <c r="I144" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -4739,7 +4742,7 @@
         <v>0</v>
       </c>
       <c r="I145" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -4747,7 +4750,7 @@
         <v>37</v>
       </c>
       <c r="B146" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
       <c r="D146" t="b">
         <v>0</v>
@@ -4762,7 +4765,7 @@
         <v>0</v>
       </c>
       <c r="I146" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -4785,7 +4788,7 @@
         <v>0</v>
       </c>
       <c r="I147" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -4793,7 +4796,7 @@
         <v>37</v>
       </c>
       <c r="B148" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D148" t="b">
         <v>0</v>
@@ -4808,7 +4811,7 @@
         <v>0</v>
       </c>
       <c r="I148" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -4816,7 +4819,7 @@
         <v>37</v>
       </c>
       <c r="B149" t="s">
-        <v>159</v>
+        <v>98</v>
       </c>
       <c r="D149" t="b">
         <v>0</v>
@@ -4831,7 +4834,7 @@
         <v>0</v>
       </c>
       <c r="I149" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -4854,7 +4857,7 @@
         <v>0</v>
       </c>
       <c r="I150" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -4877,7 +4880,7 @@
         <v>0</v>
       </c>
       <c r="I151" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -4900,7 +4903,7 @@
         <v>0</v>
       </c>
       <c r="I152" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -4923,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="I153" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -4946,7 +4949,7 @@
         <v>0</v>
       </c>
       <c r="I154" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -4969,7 +4972,7 @@
         <v>0</v>
       </c>
       <c r="I155" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -4992,7 +4995,7 @@
         <v>0</v>
       </c>
       <c r="I156" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5015,7 +5018,7 @@
         <v>0</v>
       </c>
       <c r="I157" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5038,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="I158" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -5061,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="I159" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5084,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="I160" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5107,7 +5110,7 @@
         <v>0</v>
       </c>
       <c r="I161" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5115,7 +5118,7 @@
         <v>37</v>
       </c>
       <c r="B162" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="D162" t="b">
         <v>0</v>
@@ -5130,7 +5133,30 @@
         <v>0</v>
       </c>
       <c r="I162" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="A163" t="s">
+        <v>37</v>
+      </c>
+      <c r="B163" t="s">
+        <v>124</v>
+      </c>
+      <c r="D163" t="b">
+        <v>0</v>
+      </c>
+      <c r="E163" t="b">
+        <v>0</v>
+      </c>
+      <c r="F163" t="b">
+        <v>1</v>
+      </c>
+      <c r="G163" t="b">
+        <v>0</v>
+      </c>
+      <c r="I163" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -5148,128 +5174,128 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>199</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>226</v>
       </c>
       <c r="E2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
         <v>226</v>
       </c>
       <c r="E4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" location="isAssociatedWith"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3" location="isAssociatedWith"/>
-    <hyperlink ref="C4" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5" location="isAssociatedWith"/>
-    <hyperlink ref="C5" r:id="rId6"/>
-    <hyperlink ref="F5" r:id="rId7" location="isAssociatedWith"/>
-    <hyperlink ref="C6" r:id="rId8"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2" location="isAssociatedWith"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4" location="isAssociatedWith"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="F4" r:id="rId6" location="isAssociatedWith"/>
+    <hyperlink ref="C5" r:id="rId7"/>
+    <hyperlink ref="F5" r:id="rId8" location="isAssociatedWith"/>
     <hyperlink ref="F6" r:id="rId9" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: changed data type to text
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -688,10 +688,10 @@
     <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
     <t>http://semanticscience.org/resource/SIO_001330</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
@@ -2041,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -5214,16 +5214,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E3" t="s">
         <v>228</v>
@@ -5234,16 +5234,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E4" t="s">
         <v>228</v>
@@ -5254,16 +5248,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E5" t="s">
         <v>228</v>
@@ -5274,10 +5268,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>195</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" t="s">
+        <v>226</v>
       </c>
       <c r="E6" t="s">
         <v>228</v>
@@ -5292,10 +5292,10 @@
     <hyperlink ref="F2" r:id="rId2" location="isAssociatedWith"/>
     <hyperlink ref="C3" r:id="rId3"/>
     <hyperlink ref="F3" r:id="rId4" location="isAssociatedWith"/>
-    <hyperlink ref="C4" r:id="rId5"/>
-    <hyperlink ref="F4" r:id="rId6" location="isAssociatedWith"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="F5" r:id="rId8" location="isAssociatedWith"/>
+    <hyperlink ref="F4" r:id="rId5" location="isAssociatedWith"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="F5" r:id="rId7" location="isAssociatedWith"/>
+    <hyperlink ref="C6" r:id="rId8"/>
     <hyperlink ref="F6" r:id="rId9" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjusted emx packages and attributes
</commit_message>
<xml_diff>
--- a/dist/cosasportal.xlsx
+++ b/dist/cosasportal.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="235">
   <si>
     <t>cosasportal</t>
   </si>
@@ -682,19 +682,19 @@
     <t>partOfAttribute</t>
   </si>
   <si>
-    <t>ProcessedData https://w3id.org/reproduceme#ProcessedData</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+    <t>https://w3id.org/reproduceme#ProcessedData</t>
   </si>
   <si>
     <t>http://semanticscience.org/resource/SIO_001330</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
   </si>
   <si>
     <t>NCIT</t>
@@ -5194,13 +5194,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
         <v>226</v>
@@ -5214,13 +5214,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3" t="s">
         <v>226</v>
@@ -5234,10 +5234,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>199</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" t="s">
+        <v>226</v>
       </c>
       <c r="E4" t="s">
         <v>228</v>
@@ -5248,16 +5254,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="E5" t="s">
         <v>228</v>
@@ -5268,16 +5274,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>225</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E6" t="s">
         <v>228</v>
@@ -5292,11 +5298,12 @@
     <hyperlink ref="F2" r:id="rId2" location="isAssociatedWith"/>
     <hyperlink ref="C3" r:id="rId3"/>
     <hyperlink ref="F3" r:id="rId4" location="isAssociatedWith"/>
-    <hyperlink ref="F4" r:id="rId5" location="isAssociatedWith"/>
-    <hyperlink ref="C5" r:id="rId6"/>
-    <hyperlink ref="F5" r:id="rId7" location="isAssociatedWith"/>
-    <hyperlink ref="C6" r:id="rId8"/>
-    <hyperlink ref="F6" r:id="rId9" location="isAssociatedWith"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="F4" r:id="rId6" location="isAssociatedWith"/>
+    <hyperlink ref="C5" r:id="rId7" location="ProcessedData"/>
+    <hyperlink ref="F5" r:id="rId8" location="isAssociatedWith"/>
+    <hyperlink ref="C6" r:id="rId9"/>
+    <hyperlink ref="F6" r:id="rId10" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>